<commit_message>
saved new productivity data
</commit_message>
<xml_diff>
--- a/data/Environmental/BBtotalRunFigure_2022.xlsx
+++ b/data/Environmental/BBtotalRunFigure_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracehenry/Documents/GitHub/CSIA_lab_work/data/Environmental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A22234FC-6E87-6044-9FE0-8D625EEDA55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85112461-F8F7-9B4D-B2C0-A8134494A3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="14020" activeTab="1" xr2:uid="{20C0DC70-BB3E-1145-B5ED-56A1D4888114}"/>
+    <workbookView xWindow="1920" yWindow="1420" windowWidth="23260" windowHeight="14020" activeTab="1" xr2:uid="{20C0DC70-BB3E-1145-B5ED-56A1D4888114}"/>
   </bookViews>
   <sheets>
     <sheet name="BB catch and esc (newValues (2)" sheetId="3" r:id="rId1"/>
@@ -261,10 +261,10 @@
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -584,9 +584,9 @@
   <dimension ref="A2:AX71"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1480" activePane="bottomLeft"/>
+      <pane ySplit="1480" topLeftCell="A33" activePane="bottomLeft"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="AJ9" sqref="AJ9"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1014,7 +1014,7 @@
         <v>1305818.316137434</v>
       </c>
       <c r="AI7" s="8">
-        <f t="shared" ref="AI6:AI37" si="3">Y7</f>
+        <f t="shared" ref="AI7:AI37" si="3">Y7</f>
         <v>355426.28524743248</v>
       </c>
       <c r="AJ7" s="13">
@@ -9302,2085 +9302,2158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A46595-8C2B-E846-BEDB-2805D80C5250}">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="11" width="10.83203125" style="17"/>
+    <col min="1" max="1" width="11" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="17" t="s">
-        <v>14</v>
+      <c r="K1" s="16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="19">
         <v>1963</v>
       </c>
-      <c r="B2" s="6">
-        <v>136350.69732642113</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1597997.2656147075</v>
-      </c>
-      <c r="D2" s="6">
-        <v>452397.6723727003</v>
-      </c>
-      <c r="E2" s="6">
-        <v>615338.55230864522</v>
-      </c>
-      <c r="F2" s="6">
-        <v>378138.28097299795</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1796531.008315667</v>
-      </c>
-      <c r="H2" s="6">
-        <v>1991859.7731033009</v>
-      </c>
-      <c r="I2" s="6">
-        <v>679649.32328747644</v>
-      </c>
-      <c r="J2" s="18">
-        <f>SUM(H2:I2)</f>
-        <v>2671509.0963907773</v>
-      </c>
-      <c r="K2" s="19">
-        <f>SUM(B2:J2)</f>
-        <v>10319771.669692693</v>
+      <c r="B2" s="16">
+        <v>136350.69733242318</v>
+      </c>
+      <c r="C2" s="16">
+        <v>1597997.2654902888</v>
+      </c>
+      <c r="D2" s="16">
+        <v>452397.67236674286</v>
+      </c>
+      <c r="E2" s="16">
+        <v>615338.55230708909</v>
+      </c>
+      <c r="F2" s="16">
+        <v>378138.28099703789</v>
+      </c>
+      <c r="G2" s="16">
+        <v>1796531.0083256206</v>
+      </c>
+      <c r="H2" s="16">
+        <v>1991859.7731253328</v>
+      </c>
+      <c r="I2" s="16">
+        <v>679649.32328383741</v>
+      </c>
+      <c r="J2" s="17">
+        <v>352718</v>
+      </c>
+      <c r="K2" s="16">
+        <v>8000980.5732283723</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="19">
         <v>1964</v>
       </c>
-      <c r="B3" s="6">
-        <v>191054.08969297074</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2413804.4789597308</v>
-      </c>
-      <c r="D3" s="6">
-        <v>266354.87927409576</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2181685.0606770227</v>
-      </c>
-      <c r="F3" s="6">
-        <v>759383.05037309136</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1943395.1768935914</v>
-      </c>
-      <c r="H3" s="6">
-        <v>2012601.3979868258</v>
-      </c>
-      <c r="I3" s="6">
-        <v>1305818.316137434</v>
-      </c>
-      <c r="J3" s="18">
-        <f t="shared" ref="J3:J56" si="0">SUM(H3:I3)</f>
-        <v>3318419.7141242595</v>
-      </c>
-      <c r="K3" s="19">
-        <f t="shared" ref="K3:K56" si="1">SUM(B3:J3)</f>
-        <v>14392516.16411902</v>
+      <c r="B3" s="16">
+        <v>191054.08968296894</v>
+      </c>
+      <c r="C3" s="16">
+        <v>2413804.4784538839</v>
+      </c>
+      <c r="D3" s="16">
+        <v>266354.87931409403</v>
+      </c>
+      <c r="E3" s="16">
+        <v>2181685.0606460981</v>
+      </c>
+      <c r="F3" s="16">
+        <v>759383.05031197239</v>
+      </c>
+      <c r="G3" s="16">
+        <v>1943395.1768786847</v>
+      </c>
+      <c r="H3" s="16">
+        <v>2012601.3978424701</v>
+      </c>
+      <c r="I3" s="16">
+        <v>1305818.3160628295</v>
+      </c>
+      <c r="J3" s="17">
+        <v>366342</v>
+      </c>
+      <c r="K3" s="16">
+        <v>11440438.449193001</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="19">
         <v>1965</v>
       </c>
-      <c r="B4" s="6">
-        <v>297253.0947443092</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1302507.0925220528</v>
-      </c>
-      <c r="D4" s="6">
-        <v>582186.38170118467</v>
-      </c>
-      <c r="E4" s="6">
-        <v>48627304.917333767</v>
-      </c>
-      <c r="F4" s="6">
-        <v>397860.60830266523</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1222067.3645899112</v>
-      </c>
-      <c r="H4" s="6">
-        <v>5170949.6694637891</v>
-      </c>
-      <c r="I4" s="6">
-        <v>2884254.3508556974</v>
-      </c>
-      <c r="J4" s="18">
-        <f t="shared" si="0"/>
-        <v>8055204.020319486</v>
-      </c>
-      <c r="K4" s="19">
-        <f t="shared" si="1"/>
-        <v>68539587.499832869</v>
+      <c r="B4" s="16">
+        <v>297253.0947683024</v>
+      </c>
+      <c r="C4" s="16">
+        <v>1302507.0925119042</v>
+      </c>
+      <c r="D4" s="16">
+        <v>582186.38179102144</v>
+      </c>
+      <c r="E4" s="16">
+        <v>48627304.922253482</v>
+      </c>
+      <c r="F4" s="16">
+        <v>397860.60825636447</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1222067.3645475046</v>
+      </c>
+      <c r="H4" s="16">
+        <v>5170949.6698973104</v>
+      </c>
+      <c r="I4" s="16">
+        <v>2884254.3507745671</v>
+      </c>
+      <c r="J4" s="17">
+        <v>390216</v>
+      </c>
+      <c r="K4" s="16">
+        <v>60874599.484800451</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="19">
         <v>1966</v>
       </c>
-      <c r="B5" s="6">
-        <v>310078.42211850302</v>
-      </c>
-      <c r="C5" s="6">
-        <v>2500620.8890497219</v>
-      </c>
-      <c r="D5" s="6">
-        <v>411584.84192576905</v>
-      </c>
-      <c r="E5" s="6">
-        <v>8915532.9827640951</v>
-      </c>
-      <c r="F5" s="6">
-        <v>394077.15895345696</v>
-      </c>
-      <c r="G5" s="6">
-        <v>2884786.4950709604</v>
-      </c>
-      <c r="H5" s="6">
-        <v>2903851.0501755001</v>
-      </c>
-      <c r="I5" s="6">
-        <v>1373739.2772911163</v>
-      </c>
-      <c r="J5" s="18">
-        <f t="shared" si="0"/>
-        <v>4277590.3274666164</v>
-      </c>
-      <c r="K5" s="19">
-        <f t="shared" si="1"/>
-        <v>23971861.44481574</v>
+      <c r="B5" s="16">
+        <v>310078.42211250262</v>
+      </c>
+      <c r="C5" s="16">
+        <v>2500620.8891508156</v>
+      </c>
+      <c r="D5" s="16">
+        <v>411584.84189086594</v>
+      </c>
+      <c r="E5" s="16">
+        <v>8915532.982400367</v>
+      </c>
+      <c r="F5" s="16">
+        <v>394077.15901544888</v>
+      </c>
+      <c r="G5" s="16">
+        <v>2884786.4946616003</v>
+      </c>
+      <c r="H5" s="16">
+        <v>2903851.0510047209</v>
+      </c>
+      <c r="I5" s="16">
+        <v>1373739.2773401975</v>
+      </c>
+      <c r="J5" s="17">
+        <v>338867</v>
+      </c>
+      <c r="K5" s="16">
+        <v>20033138.117576521</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="19">
         <v>1967</v>
       </c>
-      <c r="B6" s="6">
-        <v>412373.60313823761</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1150410.2062164247</v>
-      </c>
-      <c r="D6" s="6">
-        <v>139628.99250231692</v>
-      </c>
-      <c r="E6" s="6">
-        <v>5545422.5275774421</v>
-      </c>
-      <c r="F6" s="6">
-        <v>344305.5854770802</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1555050.9135648729</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1725062.7950086039</v>
-      </c>
-      <c r="I6" s="6">
-        <v>440092.796224627</v>
-      </c>
-      <c r="J6" s="18">
-        <f t="shared" si="0"/>
-        <v>2165155.5912332311</v>
-      </c>
-      <c r="K6" s="19">
-        <f t="shared" si="1"/>
-        <v>13477503.010942835</v>
+      <c r="B6" s="16">
+        <v>412373.60309748858</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1150410.2062263526</v>
+      </c>
+      <c r="D6" s="16">
+        <v>139628.99251433852</v>
+      </c>
+      <c r="E6" s="16">
+        <v>5545422.5275684744</v>
+      </c>
+      <c r="F6" s="16">
+        <v>344305.58557739743</v>
+      </c>
+      <c r="G6" s="16">
+        <v>1555050.9136540752</v>
+      </c>
+      <c r="H6" s="16">
+        <v>1725062.7950024188</v>
+      </c>
+      <c r="I6" s="16">
+        <v>440092.79616245127</v>
+      </c>
+      <c r="J6" s="17">
+        <v>171404</v>
+      </c>
+      <c r="K6" s="16">
+        <v>11483751.419802997</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="19">
         <v>1968</v>
       </c>
-      <c r="B7" s="6">
-        <v>290685.7163660425</v>
-      </c>
-      <c r="C7" s="6">
-        <v>1547964.8903320716</v>
-      </c>
-      <c r="D7" s="6">
-        <v>218458.3534894741</v>
-      </c>
-      <c r="E7" s="6">
-        <v>3975964.096160918</v>
-      </c>
-      <c r="F7" s="6">
-        <v>314033.55735911633</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1822083.2542791804</v>
-      </c>
-      <c r="H7" s="6">
-        <v>1011976.9139948317</v>
-      </c>
-      <c r="I7" s="6">
-        <v>149356.41900445809</v>
-      </c>
-      <c r="J7" s="18">
-        <f t="shared" si="0"/>
-        <v>1161333.3329992897</v>
-      </c>
-      <c r="K7" s="19">
-        <f t="shared" si="1"/>
-        <v>10491856.533985382</v>
+      <c r="B7" s="16">
+        <v>290685.71634915867</v>
+      </c>
+      <c r="C7" s="16">
+        <v>1547964.8903326232</v>
+      </c>
+      <c r="D7" s="16">
+        <v>218458.35344657383</v>
+      </c>
+      <c r="E7" s="16">
+        <v>3975964.0960902837</v>
+      </c>
+      <c r="F7" s="16">
+        <v>314033.55737485824</v>
+      </c>
+      <c r="G7" s="16">
+        <v>1822083.2542468635</v>
+      </c>
+      <c r="H7" s="16">
+        <v>1011976.9140238469</v>
+      </c>
+      <c r="I7" s="16">
+        <v>149356.41900423219</v>
+      </c>
+      <c r="J7" s="17">
+        <v>135862</v>
+      </c>
+      <c r="K7" s="16">
+        <v>9466385.2008684408</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="19">
         <v>1969</v>
       </c>
-      <c r="B8" s="6">
-        <v>759994.23045223532</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1351285.1734297215</v>
-      </c>
-      <c r="D8" s="6">
-        <v>184391.56512615204</v>
-      </c>
-      <c r="E8" s="6">
-        <v>14054748.965971155</v>
-      </c>
-      <c r="F8" s="6">
-        <v>324288.95516731887</v>
-      </c>
-      <c r="G8" s="6">
-        <v>2641101.3192682569</v>
-      </c>
-      <c r="H8" s="6">
-        <v>2016715.5004744299</v>
-      </c>
-      <c r="I8" s="6">
-        <v>301894.30163719837</v>
-      </c>
-      <c r="J8" s="18">
-        <f t="shared" si="0"/>
-        <v>2318609.8021116285</v>
-      </c>
-      <c r="K8" s="19">
-        <f t="shared" si="1"/>
-        <v>23953029.813638099</v>
+      <c r="B8" s="16">
+        <v>759994.23044126283</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1351285.1733298146</v>
+      </c>
+      <c r="D8" s="16">
+        <v>184391.56512249215</v>
+      </c>
+      <c r="E8" s="16">
+        <v>14054748.965883151</v>
+      </c>
+      <c r="F8" s="16">
+        <v>324288.95516926405</v>
+      </c>
+      <c r="G8" s="16">
+        <v>2641101.3196530957</v>
+      </c>
+      <c r="H8" s="16">
+        <v>2016715.5002629745</v>
+      </c>
+      <c r="I8" s="16">
+        <v>301894.30168088165</v>
+      </c>
+      <c r="J8" s="17">
+        <v>306138</v>
+      </c>
+      <c r="K8" s="16">
+        <v>21940558.011542935</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="19">
         <v>1970</v>
       </c>
-      <c r="B9" s="6">
-        <v>522005.61439761776</v>
-      </c>
-      <c r="C9" s="6">
-        <v>2238536.8509153142</v>
-      </c>
-      <c r="D9" s="6">
-        <v>865759.51453392277</v>
-      </c>
-      <c r="E9" s="6">
-        <v>34839684.718756586</v>
-      </c>
-      <c r="F9" s="6">
-        <v>500779.51146637119</v>
-      </c>
-      <c r="G9" s="6">
-        <v>2689519.0940840044</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1945368.9128448484</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1052934.4610938025</v>
-      </c>
-      <c r="J9" s="18">
-        <f t="shared" si="0"/>
-        <v>2998303.3739386508</v>
-      </c>
-      <c r="K9" s="19">
-        <f t="shared" si="1"/>
-        <v>47652892.052031122</v>
+      <c r="B9" s="16">
+        <v>522005.61433307367</v>
+      </c>
+      <c r="C9" s="16">
+        <v>2238536.8509950731</v>
+      </c>
+      <c r="D9" s="16">
+        <v>865759.5145332861</v>
+      </c>
+      <c r="E9" s="16">
+        <v>34839684.714753568</v>
+      </c>
+      <c r="F9" s="16">
+        <v>500779.5114211085</v>
+      </c>
+      <c r="G9" s="16">
+        <v>2689519.0939404629</v>
+      </c>
+      <c r="H9" s="16">
+        <v>1945368.912833361</v>
+      </c>
+      <c r="I9" s="16">
+        <v>1052934.4611137609</v>
+      </c>
+      <c r="J9" s="17">
+        <v>424470</v>
+      </c>
+      <c r="K9" s="16">
+        <v>45079058.673923694</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="19">
         <v>1971</v>
       </c>
-      <c r="B10" s="6">
-        <v>335231.2132791421</v>
-      </c>
-      <c r="C10" s="6">
-        <v>2063662.4613012087</v>
-      </c>
-      <c r="D10" s="6">
-        <v>674291.30570334056</v>
-      </c>
-      <c r="E10" s="6">
-        <v>6978106.7839142773</v>
-      </c>
-      <c r="F10" s="6">
-        <v>537293.52448527282</v>
-      </c>
-      <c r="G10" s="6">
-        <v>3658033.5727761714</v>
-      </c>
-      <c r="H10" s="6">
-        <v>1996100.3010544139</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1774596.3922390151</v>
-      </c>
-      <c r="J10" s="18">
-        <f t="shared" si="0"/>
-        <v>3770696.693293429</v>
-      </c>
-      <c r="K10" s="19">
-        <f t="shared" si="1"/>
-        <v>21788012.248046272</v>
+      <c r="B10" s="16">
+        <v>335231.21329444431</v>
+      </c>
+      <c r="C10" s="16">
+        <v>2063662.4615215722</v>
+      </c>
+      <c r="D10" s="16">
+        <v>674291.30567381869</v>
+      </c>
+      <c r="E10" s="16">
+        <v>6978106.7841524454</v>
+      </c>
+      <c r="F10" s="16">
+        <v>537293.52445327619</v>
+      </c>
+      <c r="G10" s="16">
+        <v>3658033.5728238644</v>
+      </c>
+      <c r="H10" s="16">
+        <v>1996100.3011288636</v>
+      </c>
+      <c r="I10" s="16">
+        <v>1774596.3918880553</v>
+      </c>
+      <c r="J10" s="17">
+        <v>485097</v>
+      </c>
+      <c r="K10" s="16">
+        <v>18502412.554936342</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="19">
         <v>1972</v>
       </c>
-      <c r="B11" s="6">
-        <v>127964.893812329</v>
-      </c>
-      <c r="C11" s="6">
-        <v>998549.90874507139</v>
-      </c>
-      <c r="D11" s="6">
-        <v>87174.071283259051</v>
-      </c>
-      <c r="E11" s="6">
-        <v>2132286.5783143514</v>
-      </c>
-      <c r="F11" s="6">
-        <v>302589.30714364437</v>
-      </c>
-      <c r="G11" s="6">
-        <v>1468384.3368660156</v>
-      </c>
-      <c r="H11" s="6">
-        <v>1774534.9472998471</v>
-      </c>
-      <c r="I11" s="6">
-        <v>131748.18363764076</v>
-      </c>
-      <c r="J11" s="18">
-        <f t="shared" si="0"/>
-        <v>1906283.1309374878</v>
-      </c>
-      <c r="K11" s="19">
-        <f t="shared" si="1"/>
-        <v>8929515.3580396473</v>
+      <c r="B11" s="16">
+        <v>127964.89381752907</v>
+      </c>
+      <c r="C11" s="16">
+        <v>998549.90872512467</v>
+      </c>
+      <c r="D11" s="16">
+        <v>87174.071285159051</v>
+      </c>
+      <c r="E11" s="16">
+        <v>2132286.578422538</v>
+      </c>
+      <c r="F11" s="16">
+        <v>302589.30717202049</v>
+      </c>
+      <c r="G11" s="16">
+        <v>1468384.3368653802</v>
+      </c>
+      <c r="H11" s="16">
+        <v>1774534.9473906413</v>
+      </c>
+      <c r="I11" s="16">
+        <v>131748.18357058289</v>
+      </c>
+      <c r="J11" s="17">
+        <v>176734</v>
+      </c>
+      <c r="K11" s="16">
+        <v>7199966.227248976</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="19">
         <v>1973</v>
       </c>
-      <c r="B12" s="6">
-        <v>113965.84748031905</v>
-      </c>
-      <c r="C12" s="6">
-        <v>735060.42095014837</v>
-      </c>
-      <c r="D12" s="6">
-        <v>417125.00626390171</v>
-      </c>
-      <c r="E12" s="6">
-        <v>410486.62938200065</v>
-      </c>
-      <c r="F12" s="6">
-        <v>63552.969374472901</v>
-      </c>
-      <c r="G12" s="6">
-        <v>684258.61734815279</v>
-      </c>
-      <c r="H12" s="6">
-        <v>787541.57447967818</v>
-      </c>
-      <c r="I12" s="6">
-        <v>63411.413719722303</v>
-      </c>
-      <c r="J12" s="18">
-        <f t="shared" si="0"/>
-        <v>850952.98819940048</v>
-      </c>
-      <c r="K12" s="19">
-        <f t="shared" si="1"/>
-        <v>4126355.4671977973</v>
+      <c r="B12" s="16">
+        <v>113965.84747882817</v>
+      </c>
+      <c r="C12" s="16">
+        <v>735060.42095543665</v>
+      </c>
+      <c r="D12" s="16">
+        <v>417125.00631485268</v>
+      </c>
+      <c r="E12" s="16">
+        <v>410486.62937762553</v>
+      </c>
+      <c r="F12" s="16">
+        <v>63552.969370713909</v>
+      </c>
+      <c r="G12" s="16">
+        <v>684258.61726495589</v>
+      </c>
+      <c r="H12" s="16">
+        <v>787541.57446953061</v>
+      </c>
+      <c r="I12" s="16">
+        <v>63411.413719911005</v>
+      </c>
+      <c r="J12" s="17">
+        <v>271311</v>
+      </c>
+      <c r="K12" s="16">
+        <v>3546713.4789518546</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="19">
         <v>1974</v>
       </c>
-      <c r="B13" s="6">
-        <v>430597.39757163241</v>
-      </c>
-      <c r="C13" s="6">
-        <v>2244579.1676022434</v>
-      </c>
-      <c r="D13" s="6">
-        <v>252194.8132280921</v>
-      </c>
-      <c r="E13" s="6">
-        <v>5061353.0875124494</v>
-      </c>
-      <c r="F13" s="6">
-        <v>247579.73043426967</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1474643.4770346368</v>
-      </c>
-      <c r="H13" s="6">
-        <v>1504237.231373918</v>
-      </c>
-      <c r="I13" s="6">
-        <v>66751.575432639176</v>
-      </c>
-      <c r="J13" s="18">
-        <f t="shared" si="0"/>
-        <v>1570988.8068065571</v>
-      </c>
-      <c r="K13" s="19">
-        <f t="shared" si="1"/>
-        <v>12852925.286996437</v>
+      <c r="B13" s="16">
+        <v>430597.39755932364</v>
+      </c>
+      <c r="C13" s="16">
+        <v>2244579.1681841877</v>
+      </c>
+      <c r="D13" s="16">
+        <v>252194.81315336659</v>
+      </c>
+      <c r="E13" s="16">
+        <v>5061353.0878230603</v>
+      </c>
+      <c r="F13" s="16">
+        <v>247579.73044687934</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1474643.4770341814</v>
+      </c>
+      <c r="H13" s="16">
+        <v>1504237.2313867868</v>
+      </c>
+      <c r="I13" s="16">
+        <v>66751.575428862299</v>
+      </c>
+      <c r="J13" s="17">
+        <v>238117</v>
+      </c>
+      <c r="K13" s="16">
+        <v>11520053.481016649</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="19">
         <v>1975</v>
       </c>
-      <c r="B14" s="6">
-        <v>357436.71919367521</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1773846.7725355786</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1053797.8024995027</v>
-      </c>
-      <c r="E14" s="6">
-        <v>16219630.709526502</v>
-      </c>
-      <c r="F14" s="6">
-        <v>112656.70162619422</v>
-      </c>
-      <c r="G14" s="6">
-        <v>3211149.7621374507</v>
-      </c>
-      <c r="H14" s="6">
-        <v>2238670.984185345</v>
-      </c>
-      <c r="I14" s="6">
-        <v>525564.69413776998</v>
-      </c>
-      <c r="J14" s="18">
-        <f t="shared" si="0"/>
-        <v>2764235.6783231152</v>
-      </c>
-      <c r="K14" s="19">
-        <f t="shared" si="1"/>
-        <v>28256989.824165132</v>
+      <c r="B14" s="16">
+        <v>357436.71919219481</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1773846.7725395607</v>
+      </c>
+      <c r="D14" s="16">
+        <v>1053797.8024605024</v>
+      </c>
+      <c r="E14" s="16">
+        <v>16219630.70343041</v>
+      </c>
+      <c r="F14" s="16">
+        <v>112656.70161976626</v>
+      </c>
+      <c r="G14" s="16">
+        <v>3211149.7628003834</v>
+      </c>
+      <c r="H14" s="16">
+        <v>2238670.9838634939</v>
+      </c>
+      <c r="I14" s="16">
+        <v>525564.69415821217</v>
+      </c>
+      <c r="J14" s="17">
+        <v>408258</v>
+      </c>
+      <c r="K14" s="16">
+        <v>25901012.140064526</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="19">
         <v>1976</v>
       </c>
-      <c r="B15" s="6">
-        <v>307997.32376061368</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1711906.9724723585</v>
-      </c>
-      <c r="D15" s="6">
-        <v>1083587.2499463633</v>
-      </c>
-      <c r="E15" s="6">
-        <v>3545332.45798819</v>
-      </c>
-      <c r="F15" s="6">
-        <v>157449.67069281233</v>
-      </c>
-      <c r="G15" s="6">
-        <v>3200600.0853383318</v>
-      </c>
-      <c r="H15" s="6">
-        <v>1704895.4477150873</v>
-      </c>
-      <c r="I15" s="6">
-        <v>618700.61880188901</v>
-      </c>
-      <c r="J15" s="18">
-        <f t="shared" si="0"/>
-        <v>2323596.0665169763</v>
-      </c>
-      <c r="K15" s="19">
-        <f t="shared" si="1"/>
-        <v>14654065.893232621</v>
+      <c r="B15" s="16">
+        <v>307997.32376966142</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1711906.9724785106</v>
+      </c>
+      <c r="D15" s="16">
+        <v>1083587.2499538821</v>
+      </c>
+      <c r="E15" s="16">
+        <v>3545332.4578460278</v>
+      </c>
+      <c r="F15" s="16">
+        <v>157449.67068392411</v>
+      </c>
+      <c r="G15" s="16">
+        <v>3200600.0853222352</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1704895.4481850825</v>
+      </c>
+      <c r="I15" s="16">
+        <v>618700.6188267048</v>
+      </c>
+      <c r="J15" s="17">
+        <v>545833</v>
+      </c>
+      <c r="K15" s="16">
+        <v>12876302.827066028</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="19">
         <v>1977</v>
       </c>
-      <c r="B16" s="6">
-        <v>170035.1478433758</v>
-      </c>
-      <c r="C16" s="6">
-        <v>812891.66825810121</v>
-      </c>
-      <c r="D16" s="6">
-        <v>1096783.0050078495</v>
-      </c>
-      <c r="E16" s="6">
-        <v>1675472.2523452379</v>
-      </c>
-      <c r="F16" s="6">
-        <v>234915.33421092035</v>
-      </c>
-      <c r="G16" s="6">
-        <v>2912820.4218791486</v>
-      </c>
-      <c r="H16" s="6">
-        <v>2998167.0095402785</v>
-      </c>
-      <c r="I16" s="6">
-        <v>429697.41252136935</v>
-      </c>
-      <c r="J16" s="18">
-        <f t="shared" si="0"/>
-        <v>3427864.4220616478</v>
-      </c>
-      <c r="K16" s="19">
-        <f t="shared" si="1"/>
-        <v>13758646.67366793</v>
+      <c r="B16" s="16">
+        <v>170035.14784187544</v>
+      </c>
+      <c r="C16" s="16">
+        <v>812891.66828358045</v>
+      </c>
+      <c r="D16" s="16">
+        <v>1096783.0050740498</v>
+      </c>
+      <c r="E16" s="16">
+        <v>1675472.2522378238</v>
+      </c>
+      <c r="F16" s="16">
+        <v>234915.33416411051</v>
+      </c>
+      <c r="G16" s="16">
+        <v>2912820.4223966151</v>
+      </c>
+      <c r="H16" s="16">
+        <v>2998167.0091723516</v>
+      </c>
+      <c r="I16" s="16">
+        <v>429697.41259431955</v>
+      </c>
+      <c r="J16" s="17">
+        <v>402023</v>
+      </c>
+      <c r="K16" s="16">
+        <v>10732805.251764724</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="19">
         <v>1978</v>
       </c>
-      <c r="B17" s="6">
-        <v>845205.12055182806</v>
-      </c>
-      <c r="C17" s="6">
-        <v>4706520.4878019299</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1431831.6696973944</v>
-      </c>
-      <c r="E17" s="6">
-        <v>7919094.2167818686</v>
-      </c>
-      <c r="F17" s="6">
-        <v>1110702.1545514518</v>
-      </c>
-      <c r="G17" s="6">
-        <v>2256809.7993748374</v>
-      </c>
-      <c r="H17" s="6">
-        <v>2078292.4734971658</v>
-      </c>
-      <c r="I17" s="6">
-        <v>97115.015033972479</v>
-      </c>
-      <c r="J17" s="18">
-        <f t="shared" si="0"/>
-        <v>2175407.4885311383</v>
-      </c>
-      <c r="K17" s="19">
-        <f t="shared" si="1"/>
-        <v>22620978.425821587</v>
+      <c r="B17" s="16">
+        <v>845205.12051774422</v>
+      </c>
+      <c r="C17" s="16">
+        <v>4706520.4882137831</v>
+      </c>
+      <c r="D17" s="16">
+        <v>1431831.6693948058</v>
+      </c>
+      <c r="E17" s="16">
+        <v>7919094.2165168831</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1110702.1544836808</v>
+      </c>
+      <c r="G17" s="16">
+        <v>2256809.7992713037</v>
+      </c>
+      <c r="H17" s="16">
+        <v>2078292.4740535098</v>
+      </c>
+      <c r="I17" s="16">
+        <v>97115.015029426999</v>
+      </c>
+      <c r="J17" s="17">
+        <v>770801</v>
+      </c>
+      <c r="K17" s="16">
+        <v>21216371.937481135</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="19">
         <v>1979</v>
       </c>
-      <c r="B18" s="6">
-        <v>1392465.7205293977</v>
-      </c>
-      <c r="C18" s="6">
-        <v>4185627.6897682026</v>
-      </c>
-      <c r="D18" s="6">
-        <v>1048799.6256134587</v>
-      </c>
-      <c r="E18" s="6">
-        <v>24927042.458877459</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1620186.9387866706</v>
-      </c>
-      <c r="G18" s="6">
-        <v>2826605.6331860214</v>
-      </c>
-      <c r="H18" s="6">
-        <v>2579853.1702323467</v>
-      </c>
-      <c r="I18" s="6">
-        <v>2286731.6208716445</v>
-      </c>
-      <c r="J18" s="18">
-        <f t="shared" si="0"/>
-        <v>4866584.7911039907</v>
-      </c>
-      <c r="K18" s="19">
-        <f t="shared" si="1"/>
-        <v>45733897.648969188</v>
+      <c r="B18" s="16">
+        <v>1392465.7202525253</v>
+      </c>
+      <c r="C18" s="16">
+        <v>4185627.6891684737</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1048799.6256134687</v>
+      </c>
+      <c r="E18" s="16">
+        <v>24927042.454004545</v>
+      </c>
+      <c r="F18" s="16">
+        <v>1620186.9391850217</v>
+      </c>
+      <c r="G18" s="16">
+        <v>2826605.633216077</v>
+      </c>
+      <c r="H18" s="16">
+        <v>2579853.1698369891</v>
+      </c>
+      <c r="I18" s="16">
+        <v>2286731.6205383977</v>
+      </c>
+      <c r="J18" s="17">
+        <v>615563</v>
+      </c>
+      <c r="K18" s="16">
+        <v>41482875.851815499</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="19">
         <v>1980</v>
       </c>
-      <c r="B19" s="6">
-        <v>2393480.9962551757</v>
-      </c>
-      <c r="C19" s="6">
-        <v>6143341.6067606024</v>
-      </c>
-      <c r="D19" s="6">
-        <v>5389939.167832802</v>
-      </c>
-      <c r="E19" s="6">
-        <v>37931680.058123671</v>
-      </c>
-      <c r="F19" s="6">
-        <v>855660.86241091404</v>
-      </c>
-      <c r="G19" s="6">
-        <v>5080050.2980192043</v>
-      </c>
-      <c r="H19" s="6">
-        <v>3449719.4068807815</v>
-      </c>
-      <c r="I19" s="6">
-        <v>4642573.2401048979</v>
-      </c>
-      <c r="J19" s="18">
-        <f t="shared" si="0"/>
-        <v>8092292.6469856799</v>
-      </c>
-      <c r="K19" s="19">
-        <f t="shared" si="1"/>
-        <v>73978738.283373728</v>
+      <c r="B19" s="16">
+        <v>2393480.9959997083</v>
+      </c>
+      <c r="C19" s="16">
+        <v>6143341.6077518091</v>
+      </c>
+      <c r="D19" s="16">
+        <v>5389939.1688737972</v>
+      </c>
+      <c r="E19" s="16">
+        <v>37931680.058737181</v>
+      </c>
+      <c r="F19" s="16">
+        <v>855660.86236964935</v>
+      </c>
+      <c r="G19" s="16">
+        <v>5080050.297889309</v>
+      </c>
+      <c r="H19" s="16">
+        <v>3449719.4065029612</v>
+      </c>
+      <c r="I19" s="16">
+        <v>4642573.2397256838</v>
+      </c>
+      <c r="J19" s="17">
+        <v>1173132</v>
+      </c>
+      <c r="K19" s="16">
+        <v>67059577.637850098</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="19">
         <v>1981</v>
       </c>
-      <c r="B20" s="6">
-        <v>1338154.4069170612</v>
-      </c>
-      <c r="C20" s="6">
-        <v>6009033.2825871017</v>
-      </c>
-      <c r="D20" s="6">
-        <v>3875793.567132635</v>
-      </c>
-      <c r="E20" s="6">
-        <v>6901353.4873204147</v>
-      </c>
-      <c r="F20" s="6">
-        <v>667234.69752736646</v>
-      </c>
-      <c r="G20" s="6">
-        <v>8756831.2367567457</v>
-      </c>
-      <c r="H20" s="6">
-        <v>4641785.1629985236</v>
-      </c>
-      <c r="I20" s="6">
-        <v>4078237.4769905712</v>
-      </c>
-      <c r="J20" s="18">
-        <f t="shared" si="0"/>
-        <v>8720022.6399890948</v>
-      </c>
-      <c r="K20" s="19">
-        <f t="shared" si="1"/>
-        <v>44988445.958219513</v>
+      <c r="B20" s="16">
+        <v>1338130.8047269615</v>
+      </c>
+      <c r="C20" s="16">
+        <v>6009033.2819866007</v>
+      </c>
+      <c r="D20" s="16">
+        <v>3875793.5670956345</v>
+      </c>
+      <c r="E20" s="16">
+        <v>6901353.4879370015</v>
+      </c>
+      <c r="F20" s="16">
+        <v>667234.69757733017</v>
+      </c>
+      <c r="G20" s="16">
+        <v>8756831.2378845531</v>
+      </c>
+      <c r="H20" s="16">
+        <v>4641785.1632384406</v>
+      </c>
+      <c r="I20" s="16">
+        <v>4078237.477049767</v>
+      </c>
+      <c r="J20" s="17">
+        <v>998636</v>
+      </c>
+      <c r="K20" s="16">
+        <v>37267035.717496291</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="19">
         <v>1982</v>
       </c>
-      <c r="B21" s="6">
-        <v>716737.27938962635</v>
-      </c>
-      <c r="C21" s="6">
-        <v>4093669.8091870314</v>
-      </c>
-      <c r="D21" s="6">
-        <v>4067177.5941901528</v>
-      </c>
-      <c r="E21" s="6">
-        <v>2811875.1392604019</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1345575.8198385264</v>
-      </c>
-      <c r="G21" s="6">
-        <v>4660805.7869137153</v>
-      </c>
-      <c r="H21" s="6">
-        <v>3785029.6762951505</v>
-      </c>
-      <c r="I21" s="6">
-        <v>2682649.7257225327</v>
-      </c>
-      <c r="J21" s="18">
-        <f t="shared" si="0"/>
-        <v>6467679.4020176828</v>
-      </c>
-      <c r="K21" s="19">
-        <f t="shared" si="1"/>
-        <v>30631200.232814819</v>
+      <c r="B21" s="16">
+        <v>716737.27936722594</v>
+      </c>
+      <c r="C21" s="16">
+        <v>4093669.809647853</v>
+      </c>
+      <c r="D21" s="16">
+        <v>4067177.5932999556</v>
+      </c>
+      <c r="E21" s="16">
+        <v>2811875.1388541921</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1345575.8198595266</v>
+      </c>
+      <c r="G21" s="16">
+        <v>4660805.7865117472</v>
+      </c>
+      <c r="H21" s="16">
+        <v>3785029.676628259</v>
+      </c>
+      <c r="I21" s="16">
+        <v>2682649.7255675346</v>
+      </c>
+      <c r="J21" s="17">
+        <v>971638</v>
+      </c>
+      <c r="K21" s="16">
+        <v>25135158.829736296</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="19">
         <v>1983</v>
       </c>
-      <c r="B22" s="6">
-        <v>1187356.7877708031</v>
-      </c>
-      <c r="C22" s="6">
-        <v>4106631.4804979851</v>
-      </c>
-      <c r="D22" s="6">
-        <v>2159923.6035259054</v>
-      </c>
-      <c r="E22" s="6">
-        <v>21496871.559681777</v>
-      </c>
-      <c r="F22" s="6">
-        <v>2664575.1777087729</v>
-      </c>
-      <c r="G22" s="6">
-        <v>3308264.2485385505</v>
-      </c>
-      <c r="H22" s="6">
-        <v>8446307.4604678508</v>
-      </c>
-      <c r="I22" s="6">
-        <v>4148448.4171679704</v>
-      </c>
-      <c r="J22" s="18">
-        <f t="shared" si="0"/>
-        <v>12594755.877635822</v>
-      </c>
-      <c r="K22" s="19">
-        <f t="shared" si="1"/>
-        <v>60113134.612995438</v>
+      <c r="B22" s="16">
+        <v>1187356.7878021041</v>
+      </c>
+      <c r="C22" s="16">
+        <v>4106631.4810955236</v>
+      </c>
+      <c r="D22" s="16">
+        <v>2159923.6034609503</v>
+      </c>
+      <c r="E22" s="16">
+        <v>21496871.565700512</v>
+      </c>
+      <c r="F22" s="16">
+        <v>2664575.1775689563</v>
+      </c>
+      <c r="G22" s="16">
+        <v>3308264.248419431</v>
+      </c>
+      <c r="H22" s="16">
+        <v>8446307.4607615545</v>
+      </c>
+      <c r="I22" s="16">
+        <v>4148448.4176983638</v>
+      </c>
+      <c r="J22" s="17">
+        <v>782718</v>
+      </c>
+      <c r="K22" s="16">
+        <v>48301096.742507398</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="19">
         <v>1984</v>
       </c>
-      <c r="B23" s="6">
-        <v>299792.02139474452</v>
-      </c>
-      <c r="C23" s="6">
-        <v>2349711.6508987918</v>
-      </c>
-      <c r="D23" s="6">
-        <v>1340820.4345760068</v>
-      </c>
-      <c r="E23" s="6">
-        <v>23930917.959976371</v>
-      </c>
-      <c r="F23" s="6">
-        <v>1193249.443101255</v>
-      </c>
-      <c r="G23" s="6">
-        <v>3876353.2655106764</v>
-      </c>
-      <c r="H23" s="6">
-        <v>5458425.1590274703</v>
-      </c>
-      <c r="I23" s="6">
-        <v>4166991.7224801872</v>
-      </c>
-      <c r="J23" s="18">
-        <f t="shared" si="0"/>
-        <v>9625416.8815076575</v>
-      </c>
-      <c r="K23" s="19">
-        <f t="shared" si="1"/>
-        <v>52241678.538473159</v>
+      <c r="B23" s="16">
+        <v>299792.02140474459</v>
+      </c>
+      <c r="C23" s="16">
+        <v>2349711.650348031</v>
+      </c>
+      <c r="D23" s="16">
+        <v>1340820.4346709638</v>
+      </c>
+      <c r="E23" s="16">
+        <v>23930917.959444489</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1193249.4434218891</v>
+      </c>
+      <c r="G23" s="16">
+        <v>3876353.2650853125</v>
+      </c>
+      <c r="H23" s="16">
+        <v>5458425.1592640411</v>
+      </c>
+      <c r="I23" s="16">
+        <v>4166991.722170745</v>
+      </c>
+      <c r="J23" s="17">
+        <v>381684</v>
+      </c>
+      <c r="K23" s="16">
+        <v>42997945.655810215</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="19">
         <v>1985</v>
       </c>
-      <c r="B24" s="6">
-        <v>643136.28298445139</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1527764.224085059</v>
-      </c>
-      <c r="D24" s="6">
-        <v>995643.31329084549</v>
-      </c>
-      <c r="E24" s="6">
-        <v>14093497.287709629</v>
-      </c>
-      <c r="F24" s="6">
-        <v>843580.10884283902</v>
-      </c>
-      <c r="G24" s="6">
-        <v>4237309.7453463078</v>
-      </c>
-      <c r="H24" s="6">
-        <v>8331666.1550605316</v>
-      </c>
-      <c r="I24" s="6">
-        <v>7940798.1985769952</v>
-      </c>
-      <c r="J24" s="18">
-        <f t="shared" si="0"/>
-        <v>16272464.353637528</v>
-      </c>
-      <c r="K24" s="19">
-        <f t="shared" si="1"/>
-        <v>54885859.669534191</v>
+      <c r="B24" s="16">
+        <v>643146.42663446232</v>
+      </c>
+      <c r="C24" s="16">
+        <v>1527764.2240861321</v>
+      </c>
+      <c r="D24" s="16">
+        <v>995643.31309076608</v>
+      </c>
+      <c r="E24" s="16">
+        <v>14093497.288607793</v>
+      </c>
+      <c r="F24" s="16">
+        <v>843580.10872609506</v>
+      </c>
+      <c r="G24" s="16">
+        <v>4237309.7456493378</v>
+      </c>
+      <c r="H24" s="16">
+        <v>8331666.155781826</v>
+      </c>
+      <c r="I24" s="16">
+        <v>7940798.1979961181</v>
+      </c>
+      <c r="J24" s="17">
+        <v>307346</v>
+      </c>
+      <c r="K24" s="16">
+        <v>38920751.460572526</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="19">
         <v>1986</v>
       </c>
-      <c r="B25" s="6">
-        <v>609140.88771199714</v>
-      </c>
-      <c r="C25" s="6">
-        <v>2106059.9512408194</v>
-      </c>
-      <c r="D25" s="6">
-        <v>2379337.9271560358</v>
-      </c>
-      <c r="E25" s="6">
-        <v>2012448.61147467</v>
-      </c>
-      <c r="F25" s="6">
-        <v>1020938.7083319169</v>
-      </c>
-      <c r="G25" s="6">
-        <v>3991315.6478098966</v>
-      </c>
-      <c r="H25" s="6">
-        <v>5506500.1318182377</v>
-      </c>
-      <c r="I25" s="6">
-        <v>6727273.6963083809</v>
-      </c>
-      <c r="J25" s="18">
-        <f t="shared" si="0"/>
-        <v>12233773.828126619</v>
-      </c>
-      <c r="K25" s="19">
-        <f t="shared" si="1"/>
-        <v>36586789.389978573</v>
+      <c r="B25" s="16">
+        <v>609140.88772109733</v>
+      </c>
+      <c r="C25" s="16">
+        <v>2106059.9512210735</v>
+      </c>
+      <c r="D25" s="16">
+        <v>2379337.9275061651</v>
+      </c>
+      <c r="E25" s="16">
+        <v>2012448.6116403597</v>
+      </c>
+      <c r="F25" s="16">
+        <v>1020938.7083222481</v>
+      </c>
+      <c r="G25" s="16">
+        <v>3991315.6484711166</v>
+      </c>
+      <c r="H25" s="16">
+        <v>5506500.1313733235</v>
+      </c>
+      <c r="I25" s="16">
+        <v>6727273.6962771947</v>
+      </c>
+      <c r="J25" s="17">
+        <v>406154</v>
+      </c>
+      <c r="K25" s="16">
+        <v>24759169.562532581</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="19">
         <v>1987</v>
       </c>
-      <c r="B26" s="6">
-        <v>471444.66453437321</v>
-      </c>
-      <c r="C26" s="6">
-        <v>3517784.9180115396</v>
-      </c>
-      <c r="D26" s="6">
-        <v>1380199.9306591568</v>
-      </c>
-      <c r="E26" s="6">
-        <v>10318113.255510923</v>
-      </c>
-      <c r="F26" s="6">
-        <v>780737.31904766359</v>
-      </c>
-      <c r="G26" s="6">
-        <v>2319010.0769531969</v>
-      </c>
-      <c r="H26" s="6">
-        <v>6385229.4437569929</v>
-      </c>
-      <c r="I26" s="6">
-        <v>2910012.7074026219</v>
-      </c>
-      <c r="J26" s="18">
-        <f t="shared" si="0"/>
-        <v>9295242.1511596143</v>
-      </c>
-      <c r="K26" s="19">
-        <f t="shared" si="1"/>
-        <v>37377774.467036083</v>
+      <c r="B26" s="16">
+        <v>471444.66451447277</v>
+      </c>
+      <c r="C26" s="16">
+        <v>3517784.9187519024</v>
+      </c>
+      <c r="D26" s="16">
+        <v>1380199.9306593766</v>
+      </c>
+      <c r="E26" s="16">
+        <v>10318113.255130306</v>
+      </c>
+      <c r="F26" s="16">
+        <v>780737.31908047292</v>
+      </c>
+      <c r="G26" s="16">
+        <v>2319010.0767258028</v>
+      </c>
+      <c r="H26" s="16">
+        <v>6385229.4437274048</v>
+      </c>
+      <c r="I26" s="16">
+        <v>2910012.707331798</v>
+      </c>
+      <c r="J26" s="17">
+        <v>573237</v>
+      </c>
+      <c r="K26" s="16">
+        <v>28655769.315921538</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="19">
         <v>1988</v>
       </c>
-      <c r="B27" s="6">
-        <v>293251.48620922648</v>
-      </c>
-      <c r="C27" s="6">
-        <v>2000001.5173264351</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1090076.2272133171</v>
-      </c>
-      <c r="E27" s="6">
-        <v>6860048.613034674</v>
-      </c>
-      <c r="F27" s="6">
-        <v>851134.59850838291</v>
-      </c>
-      <c r="G27" s="6">
-        <v>1962972.6340586408</v>
-      </c>
-      <c r="H27" s="6">
-        <v>8117564.3784150435</v>
-      </c>
-      <c r="I27" s="6">
-        <v>2155143.2117320895</v>
-      </c>
-      <c r="J27" s="18">
-        <f t="shared" si="0"/>
-        <v>10272707.590147134</v>
-      </c>
-      <c r="K27" s="19">
-        <f t="shared" si="1"/>
-        <v>33602900.256644942</v>
+      <c r="B27" s="16">
+        <v>293251.48618322611</v>
+      </c>
+      <c r="C27" s="16">
+        <v>2000001.5173192101</v>
+      </c>
+      <c r="D27" s="16">
+        <v>1090076.2272223192</v>
+      </c>
+      <c r="E27" s="16">
+        <v>6860048.6123650866</v>
+      </c>
+      <c r="F27" s="16">
+        <v>851134.59856892936</v>
+      </c>
+      <c r="G27" s="16">
+        <v>1962972.6339079791</v>
+      </c>
+      <c r="H27" s="16">
+        <v>8117564.3786909468</v>
+      </c>
+      <c r="I27" s="16">
+        <v>2155143.2116395263</v>
+      </c>
+      <c r="J27" s="17">
+        <v>1001541</v>
+      </c>
+      <c r="K27" s="16">
+        <v>24331733.665897224</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="19">
         <v>1989</v>
       </c>
-      <c r="B28" s="6">
-        <v>906594.83327758906</v>
-      </c>
-      <c r="C28" s="6">
-        <v>3099741.6349329408</v>
-      </c>
-      <c r="D28" s="6">
-        <v>1190738.0608942239</v>
-      </c>
-      <c r="E28" s="6">
-        <v>20484407.99907491</v>
-      </c>
-      <c r="F28" s="6">
-        <v>1379369.7664391596</v>
-      </c>
-      <c r="G28" s="6">
-        <v>3669831.2957043853</v>
-      </c>
-      <c r="H28" s="6">
-        <v>9807459.9929491561</v>
-      </c>
-      <c r="I28" s="6">
-        <v>5363340.071775713</v>
-      </c>
-      <c r="J28" s="18">
-        <f t="shared" si="0"/>
-        <v>15170800.06472487</v>
-      </c>
-      <c r="K28" s="19">
-        <f t="shared" si="1"/>
-        <v>61072283.71977295</v>
+      <c r="B28" s="16">
+        <v>906594.83333645738</v>
+      </c>
+      <c r="C28" s="16">
+        <v>3099741.63442238</v>
+      </c>
+      <c r="D28" s="16">
+        <v>1190738.0607803101</v>
+      </c>
+      <c r="E28" s="16">
+        <v>20484408.000472847</v>
+      </c>
+      <c r="F28" s="16">
+        <v>1379369.7665329513</v>
+      </c>
+      <c r="G28" s="16">
+        <v>3669831.2953557991</v>
+      </c>
+      <c r="H28" s="16">
+        <v>9807459.9923259951</v>
+      </c>
+      <c r="I28" s="16">
+        <v>5363340.0715971999</v>
+      </c>
+      <c r="J28" s="17">
+        <v>178895</v>
+      </c>
+      <c r="K28" s="16">
+        <v>46080378.654823937</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="19">
         <v>1990</v>
       </c>
-      <c r="B29" s="6">
-        <v>876172.31413012929</v>
-      </c>
-      <c r="C29" s="6">
-        <v>3195122.8671399122</v>
-      </c>
-      <c r="D29" s="6">
-        <v>1804526.2549877285</v>
-      </c>
-      <c r="E29" s="6">
-        <v>18192988.961009514</v>
-      </c>
-      <c r="F29" s="6">
-        <v>1591425.1865539742</v>
-      </c>
-      <c r="G29" s="6">
-        <v>8300331.6000151122</v>
-      </c>
-      <c r="H29" s="6">
-        <v>12605427.226524765</v>
-      </c>
-      <c r="I29" s="6">
-        <v>2712617.438176584</v>
-      </c>
-      <c r="J29" s="18">
-        <f t="shared" si="0"/>
-        <v>15318044.664701348</v>
-      </c>
-      <c r="K29" s="19">
-        <f t="shared" si="1"/>
-        <v>64596656.513239071</v>
+      <c r="B29" s="16">
+        <v>876172.31409093656</v>
+      </c>
+      <c r="C29" s="16">
+        <v>3195122.8662257069</v>
+      </c>
+      <c r="D29" s="16">
+        <v>1804526.2550314947</v>
+      </c>
+      <c r="E29" s="16">
+        <v>18192988.959654085</v>
+      </c>
+      <c r="F29" s="16">
+        <v>1591425.18648978</v>
+      </c>
+      <c r="G29" s="16">
+        <v>8300331.6006911239</v>
+      </c>
+      <c r="H29" s="16">
+        <v>12605427.226271007</v>
+      </c>
+      <c r="I29" s="16">
+        <v>2712617.4381450387</v>
+      </c>
+      <c r="J29" s="17">
+        <v>343722</v>
+      </c>
+      <c r="K29" s="16">
+        <v>49622333.846599177</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="19">
         <v>1991</v>
       </c>
-      <c r="B30" s="6">
-        <v>1645838.4672914408</v>
-      </c>
-      <c r="C30" s="6">
-        <v>4506270.8091147477</v>
-      </c>
-      <c r="D30" s="6">
-        <v>1628966.6271958966</v>
-      </c>
-      <c r="E30" s="6">
-        <v>8613126.7937310394</v>
-      </c>
-      <c r="F30" s="6">
-        <v>1684654.8707303482</v>
-      </c>
-      <c r="G30" s="6">
-        <v>9754424.6319379639</v>
-      </c>
-      <c r="H30" s="6">
-        <v>9235470.3279700167</v>
-      </c>
-      <c r="I30" s="6">
-        <v>5959036.3954109456</v>
-      </c>
-      <c r="J30" s="18">
-        <f t="shared" si="0"/>
-        <v>15194506.723380962</v>
-      </c>
-      <c r="K30" s="19">
-        <f t="shared" si="1"/>
-        <v>58222295.646763355</v>
+      <c r="B30" s="16">
+        <v>1645838.4675834267</v>
+      </c>
+      <c r="C30" s="16">
+        <v>4506270.8090181667</v>
+      </c>
+      <c r="D30" s="16">
+        <v>1628966.6272107321</v>
+      </c>
+      <c r="E30" s="16">
+        <v>8613126.7931583412</v>
+      </c>
+      <c r="F30" s="16">
+        <v>1684654.8706050809</v>
+      </c>
+      <c r="G30" s="16">
+        <v>9754424.6324957702</v>
+      </c>
+      <c r="H30" s="16">
+        <v>9235470.3275266942</v>
+      </c>
+      <c r="I30" s="16">
+        <v>5959036.3942727298</v>
+      </c>
+      <c r="J30" s="17">
+        <v>804954</v>
+      </c>
+      <c r="K30" s="16">
+        <v>43832742.921870939</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="19">
         <v>1992</v>
       </c>
-      <c r="B31" s="6">
-        <v>470347.57952439453</v>
-      </c>
-      <c r="C31" s="6">
-        <v>3071689.7789999098</v>
-      </c>
-      <c r="D31" s="6">
-        <v>1888874.1739033381</v>
-      </c>
-      <c r="E31" s="6">
-        <v>10628639.807809966</v>
-      </c>
-      <c r="F31" s="6">
-        <v>1461638.585831668</v>
-      </c>
-      <c r="G31" s="6">
-        <v>5222906.7843397548</v>
-      </c>
-      <c r="H31" s="6">
-        <v>17890992.667052317</v>
-      </c>
-      <c r="I31" s="6">
-        <v>6341238.5720966551</v>
-      </c>
-      <c r="J31" s="18">
-        <f t="shared" si="0"/>
-        <v>24232231.239148974</v>
-      </c>
-      <c r="K31" s="19">
-        <f t="shared" si="1"/>
-        <v>71208559.188706964</v>
+      <c r="B31" s="16">
+        <v>470347.57955026836</v>
+      </c>
+      <c r="C31" s="16">
+        <v>3071689.7790001296</v>
+      </c>
+      <c r="D31" s="16">
+        <v>1888874.17384669</v>
+      </c>
+      <c r="E31" s="16">
+        <v>10628639.806564605</v>
+      </c>
+      <c r="F31" s="16">
+        <v>1461638.5858146991</v>
+      </c>
+      <c r="G31" s="16">
+        <v>5222906.7850653362</v>
+      </c>
+      <c r="H31" s="16">
+        <v>17890992.66778025</v>
+      </c>
+      <c r="I31" s="16">
+        <v>6341238.5725719947</v>
+      </c>
+      <c r="J31" s="17">
+        <v>862258</v>
+      </c>
+      <c r="K31" s="16">
+        <v>47838585.950193971</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="19">
         <v>1993</v>
       </c>
-      <c r="B32" s="6">
-        <v>717073.20878968376</v>
-      </c>
-      <c r="C32" s="6">
-        <v>4748131.8772232393</v>
-      </c>
-      <c r="D32" s="6">
-        <v>2580049.1324144322</v>
-      </c>
-      <c r="E32" s="6">
-        <v>8064870.9293017145</v>
-      </c>
-      <c r="F32" s="6">
-        <v>2451734.914602539</v>
-      </c>
-      <c r="G32" s="6">
-        <v>5577184.7623052904</v>
-      </c>
-      <c r="H32" s="6">
-        <v>24250547.866102237</v>
-      </c>
-      <c r="I32" s="6">
-        <v>6216697.5907724816</v>
-      </c>
-      <c r="J32" s="18">
-        <f t="shared" si="0"/>
-        <v>30467245.456874721</v>
-      </c>
-      <c r="K32" s="19">
-        <f t="shared" si="1"/>
-        <v>85073535.738386333</v>
+      <c r="B32" s="16">
+        <v>717075.48643064825</v>
+      </c>
+      <c r="C32" s="16">
+        <v>4748131.8770794449</v>
+      </c>
+      <c r="D32" s="16">
+        <v>2580049.132069435</v>
+      </c>
+      <c r="E32" s="16">
+        <v>8064870.9302083431</v>
+      </c>
+      <c r="F32" s="16">
+        <v>2451734.9146045884</v>
+      </c>
+      <c r="G32" s="16">
+        <v>5577184.7624205267</v>
+      </c>
+      <c r="H32" s="16">
+        <v>24250547.860873338</v>
+      </c>
+      <c r="I32" s="16">
+        <v>6216697.5912457686</v>
+      </c>
+      <c r="J32" s="17">
+        <v>697394</v>
+      </c>
+      <c r="K32" s="16">
+        <v>55303686.554932088</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="19">
         <v>1994</v>
       </c>
-      <c r="B33" s="6">
-        <v>906804.04365063435</v>
-      </c>
-      <c r="C33" s="6">
-        <v>3696594.400909509</v>
-      </c>
-      <c r="D33" s="6">
-        <v>1436463.3012297854</v>
-      </c>
-      <c r="E33" s="6">
-        <v>21592336.781110123</v>
-      </c>
-      <c r="F33" s="6">
-        <v>2062023.39957804</v>
-      </c>
-      <c r="G33" s="6">
-        <v>3700808.2409973149</v>
-      </c>
-      <c r="H33" s="6">
-        <v>12738312.481189951</v>
-      </c>
-      <c r="I33" s="6">
-        <v>5569971.2447424205</v>
-      </c>
-      <c r="J33" s="18">
-        <f t="shared" si="0"/>
-        <v>18308283.725932371</v>
-      </c>
-      <c r="K33" s="19">
-        <f t="shared" si="1"/>
-        <v>70011597.619340152</v>
+      <c r="B33" s="16">
+        <v>906828.27085871238</v>
+      </c>
+      <c r="C33" s="16">
+        <v>3696594.4000166482</v>
+      </c>
+      <c r="D33" s="16">
+        <v>1436463.3012235884</v>
+      </c>
+      <c r="E33" s="16">
+        <v>21592336.783369124</v>
+      </c>
+      <c r="F33" s="16">
+        <v>2062023.3994319669</v>
+      </c>
+      <c r="G33" s="16">
+        <v>3700808.2410730603</v>
+      </c>
+      <c r="H33" s="16">
+        <v>12738312.480990591</v>
+      </c>
+      <c r="I33" s="16">
+        <v>5569971.2448737361</v>
+      </c>
+      <c r="J33" s="17">
+        <v>522040</v>
+      </c>
+      <c r="K33" s="16">
+        <v>52225378.12183743</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="19">
         <v>1995</v>
       </c>
-      <c r="B34" s="6">
-        <v>1184474.097597304</v>
-      </c>
-      <c r="C34" s="6">
-        <v>4938613.2230320089</v>
-      </c>
-      <c r="D34" s="6">
-        <v>810994.88798511308</v>
-      </c>
-      <c r="E34" s="6">
-        <v>28426663.092015535</v>
-      </c>
-      <c r="F34" s="6">
-        <v>2198777.9409559318</v>
-      </c>
-      <c r="G34" s="6">
-        <v>3440141.6436679871</v>
-      </c>
-      <c r="H34" s="6">
-        <v>15374929.536523942</v>
-      </c>
-      <c r="I34" s="6">
-        <v>5912957.9981985576</v>
-      </c>
-      <c r="J34" s="18">
-        <f t="shared" si="0"/>
-        <v>21287887.5347225</v>
-      </c>
-      <c r="K34" s="19">
-        <f t="shared" si="1"/>
-        <v>83575439.954698861</v>
+      <c r="B34" s="16">
+        <v>1184424.8037883053</v>
+      </c>
+      <c r="C34" s="16">
+        <v>4938613.2222320922</v>
+      </c>
+      <c r="D34" s="16">
+        <v>810994.88802611129</v>
+      </c>
+      <c r="E34" s="16">
+        <v>28426663.097102206</v>
+      </c>
+      <c r="F34" s="16">
+        <v>2198777.9406835772</v>
+      </c>
+      <c r="G34" s="16">
+        <v>3440141.6441054246</v>
+      </c>
+      <c r="H34" s="16">
+        <v>15374929.53591398</v>
+      </c>
+      <c r="I34" s="16">
+        <v>5912957.9993731249</v>
+      </c>
+      <c r="J34" s="17">
+        <v>771292</v>
+      </c>
+      <c r="K34" s="16">
+        <v>63058795.131224811</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="19">
         <v>1996</v>
       </c>
-      <c r="B35" s="6">
-        <v>942670.00950221519</v>
-      </c>
-      <c r="C35" s="6">
-        <v>5959843.735011748</v>
-      </c>
-      <c r="D35" s="6">
-        <v>1623168.6564702368</v>
-      </c>
-      <c r="E35" s="6">
-        <v>4474670.1870966218</v>
-      </c>
-      <c r="F35" s="6">
-        <v>2383541.7348524928</v>
-      </c>
-      <c r="G35" s="6">
-        <v>4662460.92687805</v>
-      </c>
-      <c r="H35" s="6">
-        <v>12416197.40843316</v>
-      </c>
-      <c r="I35" s="6">
-        <v>5370652.680410346</v>
-      </c>
-      <c r="J35" s="18">
-        <f t="shared" si="0"/>
-        <v>17786850.088843506</v>
-      </c>
-      <c r="K35" s="19">
-        <f t="shared" si="1"/>
-        <v>55620055.427498385</v>
+      <c r="B35" s="16">
+        <v>942695.89980842278</v>
+      </c>
+      <c r="C35" s="16">
+        <v>5959843.7347738585</v>
+      </c>
+      <c r="D35" s="16">
+        <v>1623168.6568484455</v>
+      </c>
+      <c r="E35" s="16">
+        <v>4474670.1871750969</v>
+      </c>
+      <c r="F35" s="16">
+        <v>2383541.7351381229</v>
+      </c>
+      <c r="G35" s="16">
+        <v>4662460.9270438524</v>
+      </c>
+      <c r="H35" s="16">
+        <v>12416197.408317542</v>
+      </c>
+      <c r="I35" s="16">
+        <v>5370652.6811896442</v>
+      </c>
+      <c r="J35" s="17">
+        <v>585899</v>
+      </c>
+      <c r="K35" s="16">
+        <v>38419130.23029498</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="19">
         <v>1997</v>
       </c>
-      <c r="B36" s="6">
-        <v>208758.54529130561</v>
-      </c>
-      <c r="C36" s="6">
-        <v>3879033.8949736478</v>
-      </c>
-      <c r="D36" s="6">
-        <v>817646.87301542528</v>
-      </c>
-      <c r="E36" s="6">
-        <v>2392217.5837767138</v>
-      </c>
-      <c r="F36" s="6">
-        <v>814336.19787836284</v>
-      </c>
-      <c r="G36" s="6">
-        <v>1910810.1955435115</v>
-      </c>
-      <c r="H36" s="6">
-        <v>7932122.5109883994</v>
-      </c>
-      <c r="I36" s="6">
-        <v>2508751.3481734716</v>
-      </c>
-      <c r="J36" s="18">
-        <f t="shared" si="0"/>
-        <v>10440873.859161871</v>
-      </c>
-      <c r="K36" s="19">
-        <f t="shared" si="1"/>
-        <v>30904551.008802712</v>
+      <c r="B36" s="16">
+        <v>208758.5452808711</v>
+      </c>
+      <c r="C36" s="16">
+        <v>3879033.8951872312</v>
+      </c>
+      <c r="D36" s="16">
+        <v>817646.87297492777</v>
+      </c>
+      <c r="E36" s="16">
+        <v>2392217.5837859306</v>
+      </c>
+      <c r="F36" s="16">
+        <v>814336.19779917644</v>
+      </c>
+      <c r="G36" s="16">
+        <v>1910810.1955949173</v>
+      </c>
+      <c r="H36" s="16">
+        <v>7932122.5097897155</v>
+      </c>
+      <c r="I36" s="16">
+        <v>2508751.3482678165</v>
+      </c>
+      <c r="J36" s="17">
+        <v>264240</v>
+      </c>
+      <c r="K36" s="16">
+        <v>20727917.148680586</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="19">
         <v>1998</v>
       </c>
-      <c r="B37" s="6">
-        <v>426033.70752241311</v>
-      </c>
-      <c r="C37" s="6">
-        <v>4421017.6574658351</v>
-      </c>
-      <c r="D37" s="6">
-        <v>991559.91839138092</v>
-      </c>
-      <c r="E37" s="6">
-        <v>3811020.5493357936</v>
-      </c>
-      <c r="F37" s="6">
-        <v>1185591.3032877957</v>
-      </c>
-      <c r="G37" s="6">
-        <v>2365116.3179727537</v>
-      </c>
-      <c r="H37" s="6">
-        <v>4689597.3507669922</v>
-      </c>
-      <c r="I37" s="6">
-        <v>1892274.6180216321</v>
-      </c>
-      <c r="J37" s="18">
-        <f t="shared" si="0"/>
-        <v>6581871.9687886238</v>
-      </c>
-      <c r="K37" s="19">
-        <f t="shared" si="1"/>
-        <v>26364083.391553219</v>
+      <c r="B37" s="16">
+        <v>426033.70753343316</v>
+      </c>
+      <c r="C37" s="16">
+        <v>4421017.6577807274</v>
+      </c>
+      <c r="D37" s="16">
+        <v>991559.91839066846</v>
+      </c>
+      <c r="E37" s="16">
+        <v>3811020.5499279462</v>
+      </c>
+      <c r="F37" s="16">
+        <v>1185591.3031894441</v>
+      </c>
+      <c r="G37" s="16">
+        <v>2365116.3177929297</v>
+      </c>
+      <c r="H37" s="16">
+        <v>4689597.3514016364</v>
+      </c>
+      <c r="I37" s="16">
+        <v>1892274.617968048</v>
+      </c>
+      <c r="J37" s="17">
+        <v>313141</v>
+      </c>
+      <c r="K37" s="16">
+        <v>20095352.423984833</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="19">
         <v>1999</v>
       </c>
-      <c r="B38" s="6">
-        <v>859317.74537179922</v>
-      </c>
-      <c r="C38" s="6">
-        <v>7403081.0159414783</v>
-      </c>
-      <c r="D38" s="6">
-        <v>451807.04580852244</v>
-      </c>
-      <c r="E38" s="6">
-        <v>13203151.607310005</v>
-      </c>
-      <c r="F38" s="6">
-        <v>3028936.6501838299</v>
-      </c>
-      <c r="G38" s="6">
-        <v>4701483.5907606641</v>
-      </c>
-      <c r="H38" s="6">
-        <v>6481074.1885749828</v>
-      </c>
-      <c r="I38" s="6">
-        <v>5223880.8069812292</v>
-      </c>
-      <c r="J38" s="18">
-        <f t="shared" si="0"/>
-        <v>11704954.995556213</v>
-      </c>
-      <c r="K38" s="19">
-        <f t="shared" si="1"/>
-        <v>53057687.646488719</v>
+      <c r="B38" s="16">
+        <v>859317.7453407998</v>
+      </c>
+      <c r="C38" s="16">
+        <v>7403081.0156409331</v>
+      </c>
+      <c r="D38" s="16">
+        <v>451807.04580622254</v>
+      </c>
+      <c r="E38" s="16">
+        <v>13203151.607404865</v>
+      </c>
+      <c r="F38" s="16">
+        <v>3028936.6496273205</v>
+      </c>
+      <c r="G38" s="16">
+        <v>4701483.590427137</v>
+      </c>
+      <c r="H38" s="16">
+        <v>6481074.1881397739</v>
+      </c>
+      <c r="I38" s="16">
+        <v>5223880.8065679641</v>
+      </c>
+      <c r="J38" s="17">
+        <v>565234</v>
+      </c>
+      <c r="K38" s="16">
+        <v>41917966.648955017</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="19">
         <v>2000</v>
       </c>
-      <c r="B39" s="6">
-        <v>982740.22802599822</v>
-      </c>
-      <c r="C39" s="6">
-        <v>6540993.8395078592</v>
-      </c>
-      <c r="D39" s="6">
-        <v>1344618.2963957707</v>
-      </c>
-      <c r="E39" s="6">
-        <v>3569954.4218921652</v>
-      </c>
-      <c r="F39" s="6">
-        <v>2189166.1818002565</v>
-      </c>
-      <c r="G39" s="6">
-        <v>3967395.1973761404</v>
-      </c>
-      <c r="H39" s="6">
-        <v>8168698.9110506494</v>
-      </c>
-      <c r="I39" s="6">
-        <v>2300098.2558663213</v>
-      </c>
-      <c r="J39" s="18">
-        <f t="shared" si="0"/>
-        <v>10468797.16691697</v>
-      </c>
-      <c r="K39" s="19">
-        <f t="shared" si="1"/>
-        <v>39532462.498832129</v>
+      <c r="B39" s="16">
+        <v>982740.22802559857</v>
+      </c>
+      <c r="C39" s="16">
+        <v>6541118.4443876632</v>
+      </c>
+      <c r="D39" s="16">
+        <v>1344618.2963997698</v>
+      </c>
+      <c r="E39" s="16">
+        <v>3569959.4210411096</v>
+      </c>
+      <c r="F39" s="16">
+        <v>2189169.9536476769</v>
+      </c>
+      <c r="G39" s="16">
+        <v>3967486.1082984773</v>
+      </c>
+      <c r="H39" s="16">
+        <v>8168699.0460164901</v>
+      </c>
+      <c r="I39" s="16">
+        <v>2300098.2883485002</v>
+      </c>
+      <c r="J39" s="17">
+        <v>1126843</v>
+      </c>
+      <c r="K39" s="16">
+        <v>30190732.786165286</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="19">
         <v>2001</v>
       </c>
-      <c r="B40" s="6">
-        <v>818733.37201707135</v>
-      </c>
-      <c r="C40" s="6">
-        <v>4644098.5787266297</v>
-      </c>
-      <c r="D40" s="6">
-        <v>2093784.9070695094</v>
-      </c>
-      <c r="E40" s="6">
-        <v>1940224.7078980133</v>
-      </c>
-      <c r="F40" s="6">
-        <v>1186912.5550045418</v>
-      </c>
-      <c r="G40" s="6">
-        <v>5991184.9401163571</v>
-      </c>
-      <c r="H40" s="6">
-        <v>3566444.1786382277</v>
-      </c>
-      <c r="I40" s="6">
-        <v>1467574.9623623735</v>
-      </c>
-      <c r="J40" s="18">
-        <f t="shared" si="0"/>
-        <v>5034019.1410006015</v>
-      </c>
-      <c r="K40" s="19">
-        <f t="shared" si="1"/>
-        <v>26742977.342833329</v>
+      <c r="B40" s="16">
+        <v>818733.37201747124</v>
+      </c>
+      <c r="C40" s="16">
+        <v>4644098.5776573112</v>
+      </c>
+      <c r="D40" s="16">
+        <v>2093784.906940555</v>
+      </c>
+      <c r="E40" s="16">
+        <v>1940224.7083412486</v>
+      </c>
+      <c r="F40" s="16">
+        <v>1186912.554952061</v>
+      </c>
+      <c r="G40" s="16">
+        <v>5991184.94059195</v>
+      </c>
+      <c r="H40" s="16">
+        <v>3566444.178967467</v>
+      </c>
+      <c r="I40" s="16">
+        <v>1467574.9624020467</v>
+      </c>
+      <c r="J40" s="17">
+        <v>1109140</v>
+      </c>
+      <c r="K40" s="16">
+        <v>22818098.20187011</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="19">
         <v>2002</v>
       </c>
-      <c r="B41" s="6">
-        <v>199681.40039931424</v>
-      </c>
-      <c r="C41" s="6">
-        <v>3859833.0937953433</v>
-      </c>
-      <c r="D41" s="6">
-        <v>691785.04486241296</v>
-      </c>
-      <c r="E41" s="6">
-        <v>897873.61099505459</v>
-      </c>
-      <c r="F41" s="6">
-        <v>941300.53288360161</v>
-      </c>
-      <c r="G41" s="6">
-        <v>2813597.6573911021</v>
-      </c>
-      <c r="H41" s="6">
-        <v>5544321.6735393694</v>
-      </c>
-      <c r="I41" s="6">
-        <v>2499048.6120604826</v>
-      </c>
-      <c r="J41" s="18">
-        <f t="shared" si="0"/>
-        <v>8043370.285599852</v>
-      </c>
-      <c r="K41" s="19">
-        <f t="shared" si="1"/>
-        <v>25490811.911526531</v>
+      <c r="B41" s="16">
+        <v>199683.67901151432</v>
+      </c>
+      <c r="C41" s="16">
+        <v>3859721.5449044663</v>
+      </c>
+      <c r="D41" s="16">
+        <v>691785.04488041322</v>
+      </c>
+      <c r="E41" s="16">
+        <v>897873.61103912571</v>
+      </c>
+      <c r="F41" s="16">
+        <v>941300.53276682727</v>
+      </c>
+      <c r="G41" s="16">
+        <v>2813597.657477363</v>
+      </c>
+      <c r="H41" s="16">
+        <v>5544321.6731135575</v>
+      </c>
+      <c r="I41" s="16">
+        <v>2499048.611998721</v>
+      </c>
+      <c r="J41" s="17">
+        <v>406290</v>
+      </c>
+      <c r="K41" s="16">
+        <v>17853622.355191987</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="19">
         <v>2003</v>
       </c>
-      <c r="B42" s="6">
-        <v>492184.31270475197</v>
-      </c>
-      <c r="C42" s="6">
-        <v>6233371.9191684229</v>
-      </c>
-      <c r="D42" s="6">
-        <v>2409659.6680879346</v>
-      </c>
-      <c r="E42" s="6">
-        <v>2001774.8234250864</v>
-      </c>
-      <c r="F42" s="6">
-        <v>4157785.6451066956</v>
-      </c>
-      <c r="G42" s="6">
-        <v>4861575.0695580114</v>
-      </c>
-      <c r="H42" s="6">
-        <v>3217355.0995870451</v>
-      </c>
-      <c r="I42" s="6">
-        <v>2540239.5830404437</v>
-      </c>
-      <c r="J42" s="18">
-        <f t="shared" si="0"/>
-        <v>5757594.6826274889</v>
-      </c>
-      <c r="K42" s="19">
-        <f t="shared" si="1"/>
-        <v>31671540.803305879</v>
+      <c r="B42" s="16">
+        <v>492184.3127045529</v>
+      </c>
+      <c r="C42" s="16">
+        <v>6233371.91952415</v>
+      </c>
+      <c r="D42" s="16">
+        <v>2409659.6682980005</v>
+      </c>
+      <c r="E42" s="16">
+        <v>2001790.1087256607</v>
+      </c>
+      <c r="F42" s="16">
+        <v>4157797.178887459</v>
+      </c>
+      <c r="G42" s="16">
+        <v>4861853.0256390143</v>
+      </c>
+      <c r="H42" s="16">
+        <v>3217355.511775271</v>
+      </c>
+      <c r="I42" s="16">
+        <v>2540239.6818193728</v>
+      </c>
+      <c r="J42" s="17">
+        <v>897566</v>
+      </c>
+      <c r="K42" s="16">
+        <v>26811817.40737348</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="19">
         <v>2004</v>
       </c>
-      <c r="B43" s="6">
-        <v>268353.82221035834</v>
-      </c>
-      <c r="C43" s="6">
-        <v>6430417.4619590091</v>
-      </c>
-      <c r="D43" s="6">
-        <v>2062468.6822873037</v>
-      </c>
-      <c r="E43" s="6">
-        <v>8091208.1666172007</v>
-      </c>
-      <c r="F43" s="6">
-        <v>7525883.7859267443</v>
-      </c>
-      <c r="G43" s="6">
-        <v>4066682.0597944199</v>
-      </c>
-      <c r="H43" s="6">
-        <v>11642565.168682534</v>
-      </c>
-      <c r="I43" s="6">
-        <v>4202790.6724684648</v>
-      </c>
-      <c r="J43" s="18">
-        <f t="shared" si="0"/>
-        <v>15845355.841150999</v>
-      </c>
-      <c r="K43" s="19">
-        <f t="shared" si="1"/>
-        <v>60135725.661097035</v>
+      <c r="B43" s="16">
+        <v>268353.82227293908</v>
+      </c>
+      <c r="C43" s="16">
+        <v>6430417.4616080439</v>
+      </c>
+      <c r="D43" s="16">
+        <v>2062468.6831826151</v>
+      </c>
+      <c r="E43" s="16">
+        <v>8091208.1660909653</v>
+      </c>
+      <c r="F43" s="16">
+        <v>7525883.7856868953</v>
+      </c>
+      <c r="G43" s="16">
+        <v>4066682.0592561662</v>
+      </c>
+      <c r="H43" s="16">
+        <v>11642565.167695941</v>
+      </c>
+      <c r="I43" s="16">
+        <v>4202790.6725382963</v>
+      </c>
+      <c r="J43" s="17">
+        <v>507677</v>
+      </c>
+      <c r="K43" s="16">
+        <v>44798046.81833186</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="19">
         <v>2005</v>
       </c>
-      <c r="B44" s="6">
-        <v>801087.32944720739</v>
-      </c>
-      <c r="C44" s="6">
-        <v>5881534.4254879728</v>
-      </c>
-      <c r="D44" s="6">
-        <v>3672976.3022932862</v>
-      </c>
-      <c r="E44" s="6">
-        <v>2867678.8883390613</v>
-      </c>
-      <c r="F44" s="6">
-        <v>5224715.5794262886</v>
-      </c>
-      <c r="G44" s="6">
-        <v>8765371.0020919107</v>
-      </c>
-      <c r="H44" s="6">
-        <v>9402204.3931682222</v>
-      </c>
-      <c r="I44" s="6">
-        <v>3090001.9504551524</v>
-      </c>
-      <c r="J44" s="18">
-        <f t="shared" si="0"/>
-        <v>12492206.343623374</v>
-      </c>
-      <c r="K44" s="19">
-        <f t="shared" si="1"/>
-        <v>52197776.214332476</v>
+      <c r="B44" s="16">
+        <v>801087.32919925079</v>
+      </c>
+      <c r="C44" s="16">
+        <v>5881534.4257071419</v>
+      </c>
+      <c r="D44" s="16">
+        <v>3672976.3020962868</v>
+      </c>
+      <c r="E44" s="16">
+        <v>2867678.8885957263</v>
+      </c>
+      <c r="F44" s="16">
+        <v>5224715.5792458653</v>
+      </c>
+      <c r="G44" s="16">
+        <v>8765371.0062913168</v>
+      </c>
+      <c r="H44" s="16">
+        <v>9402204.3922494669</v>
+      </c>
+      <c r="I44" s="16">
+        <v>3090001.9501557467</v>
+      </c>
+      <c r="J44" s="17">
+        <v>581328</v>
+      </c>
+      <c r="K44" s="16">
+        <v>40286897.873540796</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="19">
         <v>2006</v>
       </c>
-      <c r="B45" s="6">
-        <v>727744.17236943543</v>
-      </c>
-      <c r="C45" s="6">
-        <v>12640215.192163447</v>
-      </c>
-      <c r="D45" s="6">
-        <v>2731826.2703935141</v>
-      </c>
-      <c r="E45" s="6">
-        <v>5715389.7954033194</v>
-      </c>
-      <c r="F45" s="6">
-        <v>3342878.9169975282</v>
-      </c>
-      <c r="G45" s="6">
-        <v>5342241.0851752721</v>
-      </c>
-      <c r="H45" s="6">
-        <v>8613841.9371439032</v>
-      </c>
-      <c r="I45" s="6">
-        <v>3779176.1273961915</v>
-      </c>
-      <c r="J45" s="18">
-        <f t="shared" si="0"/>
-        <v>12393018.064540096</v>
-      </c>
-      <c r="K45" s="19">
-        <f t="shared" si="1"/>
-        <v>55286331.561582707</v>
+      <c r="B45" s="16">
+        <v>727744.17240243533</v>
+      </c>
+      <c r="C45" s="16">
+        <v>12640215.191230638</v>
+      </c>
+      <c r="D45" s="16">
+        <v>2731826.2707312158</v>
+      </c>
+      <c r="E45" s="16">
+        <v>5715389.7961070649</v>
+      </c>
+      <c r="F45" s="16">
+        <v>3342878.9177765865</v>
+      </c>
+      <c r="G45" s="16">
+        <v>5342241.0853943238</v>
+      </c>
+      <c r="H45" s="16">
+        <v>8613841.9371849336</v>
+      </c>
+      <c r="I45" s="16">
+        <v>3779176.1272211075</v>
+      </c>
+      <c r="J45" s="17">
+        <v>906036</v>
+      </c>
+      <c r="K45" s="16">
+        <v>43799349.498048298</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="19">
         <v>2007</v>
       </c>
-      <c r="B46" s="6">
-        <v>1022674.9621745443</v>
-      </c>
-      <c r="C46" s="6">
-        <v>7794243.466474453</v>
-      </c>
-      <c r="D46" s="6">
-        <v>2469463.1050718091</v>
-      </c>
-      <c r="E46" s="6">
-        <v>5917491.9639838208</v>
-      </c>
-      <c r="F46" s="6">
-        <v>4771232.6832998479</v>
-      </c>
-      <c r="G46" s="6">
-        <v>8438491.6768147182</v>
-      </c>
-      <c r="H46" s="6">
-        <v>7395032.4165154062</v>
-      </c>
-      <c r="I46" s="6">
-        <v>7399703.2463161591</v>
-      </c>
-      <c r="J46" s="18">
-        <f t="shared" si="0"/>
-        <v>14794735.662831565</v>
-      </c>
-      <c r="K46" s="19">
-        <f t="shared" si="1"/>
-        <v>60003069.183482319</v>
+      <c r="B46" s="16">
+        <v>1022674.9622015465</v>
+      </c>
+      <c r="C46" s="16">
+        <v>7794243.4667124599</v>
+      </c>
+      <c r="D46" s="16">
+        <v>2469463.1055957838</v>
+      </c>
+      <c r="E46" s="16">
+        <v>5917491.9633896733</v>
+      </c>
+      <c r="F46" s="16">
+        <v>4771232.6823479496</v>
+      </c>
+      <c r="G46" s="16">
+        <v>8438491.6733139418</v>
+      </c>
+      <c r="H46" s="16">
+        <v>7395032.4161607698</v>
+      </c>
+      <c r="I46" s="16">
+        <v>7399703.2451192578</v>
+      </c>
+      <c r="J46" s="17">
+        <v>1066972</v>
+      </c>
+      <c r="K46" s="16">
+        <v>46275305.514841378</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="19">
         <v>2008</v>
       </c>
-      <c r="B47" s="6">
-        <v>1888898.4928249281</v>
-      </c>
-      <c r="C47" s="6">
-        <v>6802770.1371317944</v>
-      </c>
-      <c r="D47" s="6">
-        <v>1908900.7730154255</v>
-      </c>
-      <c r="E47" s="6">
-        <v>6030619.599346213</v>
-      </c>
-      <c r="F47" s="6">
-        <v>4704660.3115661489</v>
-      </c>
-      <c r="G47" s="6">
-        <v>9127187.8114579469</v>
-      </c>
-      <c r="H47" s="6">
-        <v>7825252.2516780151</v>
-      </c>
-      <c r="I47" s="6">
-        <v>2929894.7102136551</v>
-      </c>
-      <c r="J47" s="18">
-        <f t="shared" si="0"/>
-        <v>10755146.96189167</v>
-      </c>
-      <c r="K47" s="19">
-        <f t="shared" si="1"/>
-        <v>51973331.049125791</v>
+      <c r="B47" s="16">
+        <v>1888898.492914408</v>
+      </c>
+      <c r="C47" s="16">
+        <v>6802770.1380307879</v>
+      </c>
+      <c r="D47" s="16">
+        <v>1908900.7728585186</v>
+      </c>
+      <c r="E47" s="16">
+        <v>6030619.5991111062</v>
+      </c>
+      <c r="F47" s="16">
+        <v>4704660.3112117937</v>
+      </c>
+      <c r="G47" s="16">
+        <v>9127187.8108681347</v>
+      </c>
+      <c r="H47" s="16">
+        <v>7825252.2518323911</v>
+      </c>
+      <c r="I47" s="16">
+        <v>2929894.7108458043</v>
+      </c>
+      <c r="J47" s="17">
+        <v>868540</v>
+      </c>
+      <c r="K47" s="16">
+        <v>42086724.087672949</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="19">
         <v>2009</v>
       </c>
-      <c r="B48" s="6">
-        <v>1585347.9934350071</v>
-      </c>
-      <c r="C48" s="6">
-        <v>6673678.5111744469</v>
-      </c>
-      <c r="D48" s="6">
-        <v>2077745.7673045755</v>
-      </c>
-      <c r="E48" s="6">
-        <v>6961784.0943184951</v>
-      </c>
-      <c r="F48" s="6">
-        <v>2369159.9290379738</v>
-      </c>
-      <c r="G48" s="6">
-        <v>4912919.8615169432</v>
-      </c>
-      <c r="H48" s="6">
-        <v>12269670.949551037</v>
-      </c>
-      <c r="I48" s="6">
-        <v>3851254.2225637315</v>
-      </c>
-      <c r="J48" s="18">
-        <f t="shared" si="0"/>
-        <v>16120925.172114767</v>
-      </c>
-      <c r="K48" s="19">
-        <f t="shared" si="1"/>
-        <v>56822486.501016974</v>
+      <c r="B48" s="16">
+        <v>1585347.9934337013</v>
+      </c>
+      <c r="C48" s="16">
+        <v>6673678.5113654369</v>
+      </c>
+      <c r="D48" s="16">
+        <v>2077745.7672555735</v>
+      </c>
+      <c r="E48" s="16">
+        <v>6961784.0942446534</v>
+      </c>
+      <c r="F48" s="16">
+        <v>2369159.9284568848</v>
+      </c>
+      <c r="G48" s="16">
+        <v>4912919.8614532854</v>
+      </c>
+      <c r="H48" s="16">
+        <v>12269670.950218571</v>
+      </c>
+      <c r="I48" s="16">
+        <v>3851254.2225345336</v>
+      </c>
+      <c r="J48" s="17">
+        <v>856109</v>
+      </c>
+      <c r="K48" s="16">
+        <v>41557670.328962639</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="A49" s="19">
         <v>2010</v>
       </c>
-      <c r="B49" s="6">
-        <v>1407871.0899732246</v>
-      </c>
-      <c r="C49" s="6">
-        <v>8809666.8740065042</v>
-      </c>
-      <c r="D49" s="6">
-        <v>1206250.6599678167</v>
-      </c>
-      <c r="E49" s="6">
-        <v>10779329.065828236</v>
-      </c>
-      <c r="F49" s="6">
-        <v>2815554.2568587507</v>
-      </c>
-      <c r="G49" s="6">
-        <v>5436897.8991550719</v>
-      </c>
-      <c r="H49" s="6">
-        <v>5145650.2357510468</v>
-      </c>
-      <c r="I49" s="6">
-        <v>4988743.5001531132</v>
-      </c>
-      <c r="J49" s="18">
-        <f t="shared" si="0"/>
-        <v>10134393.735904161</v>
-      </c>
-      <c r="K49" s="19">
-        <f t="shared" si="1"/>
-        <v>50724357.317597926</v>
+      <c r="B49" s="16">
+        <v>1407871.090007185</v>
+      </c>
+      <c r="C49" s="16">
+        <v>8809666.8734829798</v>
+      </c>
+      <c r="D49" s="16">
+        <v>1206250.6600049837</v>
+      </c>
+      <c r="E49" s="16">
+        <v>10779329.06665319</v>
+      </c>
+      <c r="F49" s="16">
+        <v>2815554.2563738255</v>
+      </c>
+      <c r="G49" s="16">
+        <v>5436897.8995730774</v>
+      </c>
+      <c r="H49" s="16">
+        <v>5145650.236255439</v>
+      </c>
+      <c r="I49" s="16">
+        <v>4988743.4998507518</v>
+      </c>
+      <c r="J49" s="17">
+        <v>641004</v>
+      </c>
+      <c r="K49" s="16">
+        <v>41230967.582201436</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="A50" s="19">
         <v>2011</v>
       </c>
-      <c r="B50" s="6">
-        <v>1015858.0737659141</v>
-      </c>
-      <c r="C50" s="6">
-        <v>4949205.8915399164</v>
-      </c>
-      <c r="D50" s="6">
-        <v>1167743.4754200825</v>
-      </c>
-      <c r="E50" s="6">
-        <v>7228364.438354725</v>
-      </c>
-      <c r="F50" s="6">
-        <v>2249301.6713185362</v>
-      </c>
-      <c r="G50" s="6">
-        <v>5520113.2305299742</v>
-      </c>
-      <c r="H50" s="6">
-        <v>4604185.0171716558</v>
-      </c>
-      <c r="I50" s="6">
-        <v>4203387.327510369</v>
-      </c>
-      <c r="J50" s="18">
-        <f t="shared" si="0"/>
-        <v>8807572.3446820248</v>
-      </c>
-      <c r="K50" s="19">
-        <f t="shared" si="1"/>
-        <v>39745731.470293194</v>
+      <c r="B50" s="16">
+        <v>1015858.0737329132</v>
+      </c>
+      <c r="C50" s="16">
+        <v>4949205.8916695118</v>
+      </c>
+      <c r="D50" s="16">
+        <v>1167743.475429052</v>
+      </c>
+      <c r="E50" s="16">
+        <v>7228364.4381130366</v>
+      </c>
+      <c r="F50" s="16">
+        <v>2249301.671423099</v>
+      </c>
+      <c r="G50" s="16">
+        <v>5520113.2306093536</v>
+      </c>
+      <c r="H50" s="16">
+        <v>4604185.0167821674</v>
+      </c>
+      <c r="I50" s="16">
+        <v>4203387.3281213315</v>
+      </c>
+      <c r="J50" s="17">
+        <v>858557</v>
+      </c>
+      <c r="K50" s="16">
+        <v>31796716.125880465</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="A51" s="19">
         <v>2012</v>
       </c>
-      <c r="B51" s="6">
-        <v>507046.12950290082</v>
-      </c>
-      <c r="C51" s="6">
-        <v>2698060.3077006349</v>
-      </c>
-      <c r="D51" s="6">
-        <v>1037757.0562016403</v>
-      </c>
-      <c r="E51" s="6">
-        <v>12263918.588477792</v>
-      </c>
-      <c r="F51" s="6">
-        <v>2226527.1482468257</v>
-      </c>
-      <c r="G51" s="6">
-        <v>3321536.1437244988</v>
-      </c>
-      <c r="H51" s="6">
-        <v>5923046.4044479216</v>
-      </c>
-      <c r="I51" s="6">
-        <v>2920818.0197462765</v>
-      </c>
-      <c r="J51" s="18">
-        <f t="shared" si="0"/>
-        <v>8843864.4241941981</v>
-      </c>
-      <c r="K51" s="19">
-        <f t="shared" si="1"/>
-        <v>39742574.222242683</v>
+      <c r="B51" s="16">
+        <v>507046.12932366162</v>
+      </c>
+      <c r="C51" s="16">
+        <v>2698060.3072247133</v>
+      </c>
+      <c r="D51" s="16">
+        <v>1037757.0561976568</v>
+      </c>
+      <c r="E51" s="16">
+        <v>12263918.588363383</v>
+      </c>
+      <c r="F51" s="16">
+        <v>2226527.1483331015</v>
+      </c>
+      <c r="G51" s="16">
+        <v>3321536.1436134288</v>
+      </c>
+      <c r="H51" s="16">
+        <v>5923046.4048542576</v>
+      </c>
+      <c r="I51" s="16">
+        <v>2920818.0197134069</v>
+      </c>
+      <c r="J51" s="17">
+        <v>832938</v>
+      </c>
+      <c r="K51" s="16">
+        <v>31731647.797623608</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52">
+      <c r="A52" s="19">
         <v>2013</v>
       </c>
-      <c r="B52" s="6">
-        <v>692485.07379958581</v>
-      </c>
-      <c r="C52" s="6">
-        <v>3286042.5272031715</v>
-      </c>
-      <c r="D52" s="6">
-        <v>2009703.6789664237</v>
-      </c>
-      <c r="E52" s="6">
-        <v>6324295.1224952852</v>
-      </c>
-      <c r="F52" s="6">
-        <v>1929766.9273869791</v>
-      </c>
-      <c r="G52" s="6">
-        <v>3074128.0689075566</v>
-      </c>
-      <c r="H52" s="6">
-        <v>5124465.512249344</v>
-      </c>
-      <c r="I52" s="6">
-        <v>2633700.2317668796</v>
-      </c>
-      <c r="J52" s="18">
-        <f t="shared" si="0"/>
-        <v>7758165.7440162236</v>
-      </c>
-      <c r="K52" s="19">
-        <f t="shared" si="1"/>
-        <v>32832752.886791445</v>
+      <c r="B52" s="16">
+        <v>692485.07366390934</v>
+      </c>
+      <c r="C52" s="16">
+        <v>3286042.527301305</v>
+      </c>
+      <c r="D52" s="16">
+        <v>2009703.6786604244</v>
+      </c>
+      <c r="E52" s="16">
+        <v>6324295.1216673674</v>
+      </c>
+      <c r="F52" s="16">
+        <v>1929766.9277610492</v>
+      </c>
+      <c r="G52" s="16">
+        <v>3074128.0685298359</v>
+      </c>
+      <c r="H52" s="16">
+        <v>5124465.5118557476</v>
+      </c>
+      <c r="I52" s="16">
+        <v>2633700.2319553443</v>
+      </c>
+      <c r="J52" s="17">
+        <v>592763</v>
+      </c>
+      <c r="K52" s="16">
+        <v>25667350.141394984</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53">
+      <c r="A53" s="19">
         <v>2014</v>
       </c>
-      <c r="B53" s="6">
-        <v>1436176.0480487132</v>
-      </c>
-      <c r="C53" s="6">
-        <v>7166061.0873729512</v>
-      </c>
-      <c r="D53" s="6">
-        <v>1510012.2100070822</v>
-      </c>
-      <c r="E53" s="6">
-        <v>17600068.186704289</v>
-      </c>
-      <c r="F53" s="6">
-        <v>1620274.2510292418</v>
-      </c>
-      <c r="G53" s="6">
-        <v>5320300.433065745</v>
-      </c>
-      <c r="H53" s="6">
-        <v>5078503.2144307699</v>
-      </c>
-      <c r="I53" s="6">
-        <v>1154016.5807186454</v>
-      </c>
-      <c r="J53" s="18">
-        <f t="shared" si="0"/>
-        <v>6232519.7951494157</v>
-      </c>
-      <c r="K53" s="19">
-        <f t="shared" si="1"/>
-        <v>47117931.806526855</v>
+      <c r="B53" s="16">
+        <v>1436176.0474854857</v>
+      </c>
+      <c r="C53" s="16">
+        <v>7166061.0865669185</v>
+      </c>
+      <c r="D53" s="16">
+        <v>1510012.2098330874</v>
+      </c>
+      <c r="E53" s="16">
+        <v>17600068.18678391</v>
+      </c>
+      <c r="F53" s="16">
+        <v>1620274.2513368665</v>
+      </c>
+      <c r="G53" s="16">
+        <v>5320300.4327192511</v>
+      </c>
+      <c r="H53" s="16">
+        <v>5078503.2145262901</v>
+      </c>
+      <c r="I53" s="16">
+        <v>1154016.5807838109</v>
+      </c>
+      <c r="J53" s="17">
+        <v>533288</v>
+      </c>
+      <c r="K53" s="16">
+        <v>41418700.010035619</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54">
+      <c r="A54" s="19">
         <v>2015</v>
       </c>
-      <c r="B54" s="6">
-        <v>1643379.1011856939</v>
-      </c>
-      <c r="C54" s="6">
-        <v>5019839.1145307422</v>
-      </c>
-      <c r="D54" s="6">
-        <v>2475985.3954162551</v>
-      </c>
-      <c r="E54" s="6">
-        <v>23104927.301168997</v>
-      </c>
-      <c r="F54" s="6">
-        <v>8244526.016329214</v>
-      </c>
-      <c r="G54" s="6">
-        <v>6090738.0293323696</v>
-      </c>
-      <c r="H54" s="6">
-        <v>8508004.3754115943</v>
-      </c>
-      <c r="I54" s="6">
-        <v>4249070.2718959022</v>
-      </c>
-      <c r="J54" s="18">
-        <f t="shared" si="0"/>
-        <v>12757074.647307497</v>
-      </c>
-      <c r="K54" s="19">
-        <f t="shared" si="1"/>
-        <v>72093544.252578259</v>
+      <c r="B54" s="16">
+        <v>1643379.1011854007</v>
+      </c>
+      <c r="C54" s="16">
+        <v>5019839.1132437298</v>
+      </c>
+      <c r="D54" s="16">
+        <v>2475985.3950491627</v>
+      </c>
+      <c r="E54" s="16">
+        <v>23104927.301222567</v>
+      </c>
+      <c r="F54" s="16">
+        <v>8244526.0167350629</v>
+      </c>
+      <c r="G54" s="16">
+        <v>6090738.0284150057</v>
+      </c>
+      <c r="H54" s="16">
+        <v>8508004.3750148974</v>
+      </c>
+      <c r="I54" s="16">
+        <v>4249070.2717489023</v>
+      </c>
+      <c r="J54" s="17">
+        <v>526750</v>
+      </c>
+      <c r="K54" s="16">
+        <v>59863219.602614731</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="A55" s="19">
         <v>2016</v>
       </c>
-      <c r="B55" s="6">
-        <v>1912626.3364949119</v>
-      </c>
-      <c r="C55" s="6">
-        <v>5382715.2001819052</v>
-      </c>
-      <c r="D55" s="6">
-        <v>3360040.8901216937</v>
-      </c>
-      <c r="E55" s="6">
-        <v>12669029.137033461</v>
-      </c>
-      <c r="F55" s="6">
-        <v>4957298.0128061986</v>
-      </c>
-      <c r="G55" s="6">
-        <v>5358303.842078262</v>
-      </c>
-      <c r="H55" s="6">
-        <v>9036510.1170837153</v>
-      </c>
-      <c r="I55" s="6">
-        <v>8831921.3923594225</v>
-      </c>
-      <c r="J55" s="18">
-        <f t="shared" si="0"/>
-        <v>17868431.509443138</v>
-      </c>
-      <c r="K55" s="19">
-        <f t="shared" si="1"/>
-        <v>69376876.437602699</v>
+      <c r="B55" s="16">
+        <v>1850333.7032025028</v>
+      </c>
+      <c r="C55" s="16">
+        <v>6384574.6289297864</v>
+      </c>
+      <c r="D55" s="16">
+        <v>2575667.3057219028</v>
+      </c>
+      <c r="E55" s="16">
+        <v>14195449.420282537</v>
+      </c>
+      <c r="F55" s="16">
+        <v>4938142.3356476547</v>
+      </c>
+      <c r="G55" s="16">
+        <v>5037024.1272555254</v>
+      </c>
+      <c r="H55" s="16">
+        <v>9891849.2478553243</v>
+      </c>
+      <c r="I55" s="16">
+        <v>7192817.5042568715</v>
+      </c>
+      <c r="J55" s="17">
+        <v>737938</v>
+      </c>
+      <c r="K55" s="16">
+        <v>52803796.273152106</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="A56" s="19">
         <v>2017</v>
       </c>
-      <c r="B56" s="6">
-        <v>1228466.9465272846</v>
-      </c>
-      <c r="C56" s="6">
-        <v>11316071.682290897</v>
-      </c>
-      <c r="D56" s="6">
-        <v>8156817.4967434527</v>
-      </c>
-      <c r="E56" s="6">
-        <v>7783315.9426815314</v>
-      </c>
-      <c r="F56" s="6">
-        <v>4800304.599116141</v>
-      </c>
-      <c r="G56" s="6">
-        <v>6514161.3408296173</v>
-      </c>
-      <c r="H56" s="6">
-        <v>12379290.976854537</v>
-      </c>
-      <c r="I56" s="6">
-        <v>6625230.0695591923</v>
-      </c>
-      <c r="J56" s="18">
-        <f t="shared" si="0"/>
-        <v>19004521.046413727</v>
-      </c>
-      <c r="K56" s="19">
-        <f t="shared" si="1"/>
-        <v>77808180.101016387</v>
+      <c r="B56" s="16">
+        <v>1230311.7189691865</v>
+      </c>
+      <c r="C56" s="16">
+        <v>11287413.550867695</v>
+      </c>
+      <c r="D56" s="16">
+        <v>8199368.3826631457</v>
+      </c>
+      <c r="E56" s="16">
+        <v>7250329.0928671798</v>
+      </c>
+      <c r="F56" s="16">
+        <v>4430315.2449948909</v>
+      </c>
+      <c r="G56" s="16">
+        <v>5975665.3718310976</v>
+      </c>
+      <c r="H56" s="16">
+        <v>12441095.332119217</v>
+      </c>
+      <c r="I56" s="16">
+        <v>6672737.5417433279</v>
+      </c>
+      <c r="J56" s="17">
+        <v>674286</v>
+      </c>
+      <c r="K56" s="16">
+        <v>58161522.236055747</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="19">
+        <v>2018</v>
+      </c>
+      <c r="B57" s="16">
+        <v>1920088.3223160806</v>
+      </c>
+      <c r="C57" s="16">
+        <v>22680172.712358359</v>
+      </c>
+      <c r="D57" s="16">
+        <v>9602178.934049774</v>
+      </c>
+      <c r="E57" s="16">
+        <v>7466680.0050265919</v>
+      </c>
+      <c r="F57" s="16">
+        <v>2873549.5305123511</v>
+      </c>
+      <c r="G57" s="16">
+        <v>6926059.981379535</v>
+      </c>
+      <c r="H57" s="16">
+        <v>6104312.171370714</v>
+      </c>
+      <c r="I57" s="16">
+        <v>4770222.7638383303</v>
+      </c>
+      <c r="J57" s="16">
+        <v>1361343</v>
+      </c>
+      <c r="K57" s="16">
+        <v>63704607.420851737</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="19">
+        <v>2019</v>
+      </c>
+      <c r="B58" s="16">
+        <v>1358926.9841471734</v>
+      </c>
+      <c r="C58" s="16">
+        <v>12340740.139324188</v>
+      </c>
+      <c r="D58" s="16">
+        <v>4306596.0689208265</v>
+      </c>
+      <c r="E58" s="16">
+        <v>7936268.7892635735</v>
+      </c>
+      <c r="F58" s="16">
+        <v>1855135.6227310856</v>
+      </c>
+      <c r="G58" s="16">
+        <v>8824530.4353730641</v>
+      </c>
+      <c r="H58" s="16">
+        <v>15434052.036566636</v>
+      </c>
+      <c r="I58" s="16">
+        <v>3604963.0527924863</v>
+      </c>
+      <c r="J58" s="16">
+        <v>1286738</v>
+      </c>
+      <c r="K58" s="16">
+        <v>56947951.129119039</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="19">
+        <v>2020</v>
+      </c>
+      <c r="B59" s="16">
+        <v>1212549.00741251</v>
+      </c>
+      <c r="C59" s="16">
+        <v>8004914.9431250533</v>
+      </c>
+      <c r="D59" s="16">
+        <v>3625516.9006801574</v>
+      </c>
+      <c r="E59" s="16">
+        <v>9866664.5977398101</v>
+      </c>
+      <c r="F59" s="16">
+        <v>4561207.9638651656</v>
+      </c>
+      <c r="G59" s="16">
+        <v>10102211.955522591</v>
+      </c>
+      <c r="H59" s="16">
+        <v>15597218.528552273</v>
+      </c>
+      <c r="I59" s="16">
+        <v>5078613.9753586585</v>
+      </c>
+      <c r="J59" s="16">
+        <v>621050</v>
+      </c>
+      <c r="K59" s="16">
+        <v>58669947.872256212</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="19">
+        <v>2021</v>
+      </c>
+      <c r="B60" s="16">
+        <v>2022716.2295807351</v>
+      </c>
+      <c r="C60" s="16">
+        <v>12667857.772416132</v>
+      </c>
+      <c r="D60" s="16">
+        <v>15070741.884804917</v>
+      </c>
+      <c r="E60" s="16">
+        <v>8885857.93250704</v>
+      </c>
+      <c r="F60" s="16">
+        <v>6069545.848240816</v>
+      </c>
+      <c r="G60" s="16">
+        <v>7095631.9946893519</v>
+      </c>
+      <c r="H60" s="16">
+        <v>7725547.0024254546</v>
+      </c>
+      <c r="I60" s="16">
+        <v>10657141.520816172</v>
+      </c>
+      <c r="J60" s="16">
+        <v>956709</v>
+      </c>
+      <c r="K60" s="16">
+        <v>71151749.185480624</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="19">
+        <v>2022</v>
+      </c>
+      <c r="B61" s="16">
+        <v>2995798.3870611056</v>
+      </c>
+      <c r="C61" s="16">
+        <v>12454475.490805157</v>
+      </c>
+      <c r="D61" s="16">
+        <v>16394969.22773567</v>
+      </c>
+      <c r="E61" s="16">
+        <v>13692831.674578745</v>
+      </c>
+      <c r="F61" s="16">
+        <v>4660506.5218241718</v>
+      </c>
+      <c r="G61" s="16">
+        <v>6475044.8489693627</v>
+      </c>
+      <c r="H61" s="16">
+        <v>18220031.553716276</v>
+      </c>
+      <c r="I61" s="16">
+        <v>7560060.4821575629</v>
+      </c>
+      <c r="J61" s="16">
+        <v>828196</v>
+      </c>
+      <c r="K61" s="16">
+        <v>83281914.186848044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>